<commit_message>
Added detailed ZA education data.
</commit_message>
<xml_diff>
--- a/data/Excel Workbooks/SUN/SUN Data with education.xlsx
+++ b/data/Excel Workbooks/SUN/SUN Data with education.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8420" yWindow="2740" windowWidth="25040" windowHeight="17000" tabRatio="500" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Indexed" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
     <author>stan</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="239">
   <si>
     <t>Year</t>
   </si>
@@ -677,9 +677,6 @@
     <t>Total formal</t>
   </si>
   <si>
-    <t>Total plus informal</t>
-  </si>
-  <si>
     <t>Total high skill</t>
   </si>
   <si>
@@ -792,6 +789,24 @@
   </si>
   <si>
     <t>Total formal with education</t>
+  </si>
+  <si>
+    <t>Total form+inf with education</t>
+  </si>
+  <si>
+    <t>Total form+inf</t>
+  </si>
+  <si>
+    <t>iL_f</t>
+  </si>
+  <si>
+    <t>iL_f+e</t>
+  </si>
+  <si>
+    <t>iL_f+i</t>
+  </si>
+  <si>
+    <t>iL_f+i+e</t>
   </si>
 </sst>
 </file>
@@ -1131,10 +1146,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1430,7 +1447,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="51">
     <cellStyle name="Comma 2" xfId="2"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1455,6 +1472,7 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -1478,6 +1496,7 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -1963,11 +1982,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2065068952"/>
-        <c:axId val="2065078168"/>
+        <c:axId val="-2146386248"/>
+        <c:axId val="-2146389208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2065068952"/>
+        <c:axId val="-2146386248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1976,7 +1995,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2065078168"/>
+        <c:crossAx val="-2146389208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1984,7 +2003,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2065078168"/>
+        <c:axId val="-2146389208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1995,7 +2014,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2065068952"/>
+        <c:crossAx val="-2146386248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2266,136 +2285,136 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="68"/>
-                <c:pt idx="24" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="24" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8.10704452777018E6</c:v>
                 </c:pt>
-                <c:pt idx="25" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="25" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8.29366185351877E6</c:v>
                 </c:pt>
-                <c:pt idx="26" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="26" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8.43936218606444E6</c:v>
                 </c:pt>
-                <c:pt idx="27" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="27" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8.78016939085434E6</c:v>
                 </c:pt>
-                <c:pt idx="28" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="28" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>9.09500061789813E6</c:v>
                 </c:pt>
-                <c:pt idx="29" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="29" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>9.37732672607092E6</c:v>
                 </c:pt>
-                <c:pt idx="30" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="30" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>9.45535836782911E6</c:v>
                 </c:pt>
-                <c:pt idx="31" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="31" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>9.32722892487701E6</c:v>
                 </c:pt>
-                <c:pt idx="32" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="32" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>9.34521694220783E6</c:v>
                 </c:pt>
-                <c:pt idx="33" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="33" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>9.4748795155029E6</c:v>
                 </c:pt>
-                <c:pt idx="34" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="34" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>9.79143880027184E6</c:v>
                 </c:pt>
-                <c:pt idx="35" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="35" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.0081385609016E7</c:v>
                 </c:pt>
-                <c:pt idx="36" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="36" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.0194221203884E7</c:v>
                 </c:pt>
-                <c:pt idx="37" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="37" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.01216252754442E7</c:v>
                 </c:pt>
-                <c:pt idx="38" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="38" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.0209330734716E7</c:v>
                 </c:pt>
-                <c:pt idx="39" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="39" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.01685593892877E7</c:v>
                 </c:pt>
-                <c:pt idx="40" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="40" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.02428412515776E7</c:v>
                 </c:pt>
-                <c:pt idx="41" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.03391097181967E7</c:v>
                 </c:pt>
-                <c:pt idx="42" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="42" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.04633940380102E7</c:v>
                 </c:pt>
-                <c:pt idx="43" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="43" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.05283301643651E7</c:v>
                 </c:pt>
-                <c:pt idx="44" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="44" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.04967480618164E7</c:v>
                 </c:pt>
-                <c:pt idx="45" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="45" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.03487116033372E7</c:v>
                 </c:pt>
-                <c:pt idx="46" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="46" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.02111878713103E7</c:v>
                 </c:pt>
-                <c:pt idx="47" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="47" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.00910951473149E7</c:v>
                 </c:pt>
-                <c:pt idx="48" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="48" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.00499274318025E7</c:v>
                 </c:pt>
-                <c:pt idx="49" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="49" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.00607171373313E7</c:v>
                 </c:pt>
-                <c:pt idx="50" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="50" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.01499826210434E7</c:v>
                 </c:pt>
-                <c:pt idx="51" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="51" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.01225423404756E7</c:v>
                 </c:pt>
-                <c:pt idx="52" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="52" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>9.97030851490526E6</c:v>
                 </c:pt>
-                <c:pt idx="53" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="53" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>9.91669042600568E6</c:v>
                 </c:pt>
-                <c:pt idx="54" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="54" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>9.83968430795629E6</c:v>
                 </c:pt>
-                <c:pt idx="55" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="55" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>9.74272828768993E6</c:v>
                 </c:pt>
-                <c:pt idx="56" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="56" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.01402605645256E7</c:v>
                 </c:pt>
-                <c:pt idx="57" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="57" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.00490282671501E7</c:v>
                 </c:pt>
-                <c:pt idx="58" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="58" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.01209959573316E7</c:v>
                 </c:pt>
-                <c:pt idx="59" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="59" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.00882351761486E7</c:v>
                 </c:pt>
-                <c:pt idx="60" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="60" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.04974059313819E7</c:v>
                 </c:pt>
-                <c:pt idx="61" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="61" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.06484181869389E7</c:v>
                 </c:pt>
-                <c:pt idx="62" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="62" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.05883194567503E7</c:v>
                 </c:pt>
-                <c:pt idx="63" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="63" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.022262106702E7</c:v>
                 </c:pt>
-                <c:pt idx="64" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="64" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.00599823197802E7</c:v>
                 </c:pt>
-                <c:pt idx="65" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="65" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.01882527465068E7</c:v>
                 </c:pt>
-                <c:pt idx="66" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="66" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.03591384402656E7</c:v>
                 </c:pt>
-                <c:pt idx="67" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="67" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.04436068593974E7</c:v>
                 </c:pt>
               </c:numCache>
@@ -2412,7 +2431,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Total plus informal</c:v>
+                  <c:v>Total form+inf</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2638,136 +2657,136 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="68"/>
-                <c:pt idx="24" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="24" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8.66046468582472E6</c:v>
                 </c:pt>
-                <c:pt idx="25" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="25" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8.91491034561097E6</c:v>
                 </c:pt>
-                <c:pt idx="26" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="26" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>9.11650351825517E6</c:v>
                 </c:pt>
-                <c:pt idx="27" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="27" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>9.51397286566277E6</c:v>
                 </c:pt>
-                <c:pt idx="28" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="28" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>9.87782984946586E6</c:v>
                 </c:pt>
-                <c:pt idx="29" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="29" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.02058355009166E7</c:v>
                 </c:pt>
-                <c:pt idx="30" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="30" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.03382923323667E7</c:v>
                 </c:pt>
-                <c:pt idx="31" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="31" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.0264164120291E7</c:v>
                 </c:pt>
-                <c:pt idx="32" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="32" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.03476350935093E7</c:v>
                 </c:pt>
-                <c:pt idx="33" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="33" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.0535394973516E7</c:v>
                 </c:pt>
-                <c:pt idx="34" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="34" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.09143960361413E7</c:v>
                 </c:pt>
-                <c:pt idx="35" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="35" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.12581079829219E7</c:v>
                 </c:pt>
-                <c:pt idx="36" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="36" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.14310224539481E7</c:v>
                 </c:pt>
-                <c:pt idx="37" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="37" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.14188453611806E7</c:v>
                 </c:pt>
-                <c:pt idx="38" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="38" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.15897590130072E7</c:v>
                 </c:pt>
-                <c:pt idx="39" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="39" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.16309079666316E7</c:v>
                 </c:pt>
-                <c:pt idx="40" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="40" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.17952020121654E7</c:v>
                 </c:pt>
-                <c:pt idx="41" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.19798944285945E7</c:v>
                 </c:pt>
-                <c:pt idx="42" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="42" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.2195578139361E7</c:v>
                 </c:pt>
-                <c:pt idx="43" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="43" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.2360770318562E7</c:v>
                 </c:pt>
-                <c:pt idx="44" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="44" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.24451350937068E7</c:v>
                 </c:pt>
-                <c:pt idx="45" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="45" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.24202931472655E7</c:v>
                 </c:pt>
-                <c:pt idx="46" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="46" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.24116411437375E7</c:v>
                 </c:pt>
-                <c:pt idx="47" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="47" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.24363815376163E7</c:v>
                 </c:pt>
-                <c:pt idx="48" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="48" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.25027960463821E7</c:v>
                 </c:pt>
-                <c:pt idx="49" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="49" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.26446081973583E7</c:v>
                 </c:pt>
-                <c:pt idx="50" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="50" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.28234177834495E7</c:v>
                 </c:pt>
-                <c:pt idx="51" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="51" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.28594908047868E7</c:v>
                 </c:pt>
-                <c:pt idx="52" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="52" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.27242602294302E7</c:v>
                 </c:pt>
-                <c:pt idx="53" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="53" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.26926155037904E7</c:v>
                 </c:pt>
-                <c:pt idx="54" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="54" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.2561482082876E7</c:v>
                 </c:pt>
-                <c:pt idx="55" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="55" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.20704263264368E7</c:v>
                 </c:pt>
-                <c:pt idx="56" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="56" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.19546914243846E7</c:v>
                 </c:pt>
-                <c:pt idx="57" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="57" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.22175466076796E7</c:v>
                 </c:pt>
-                <c:pt idx="58" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="58" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.2537828305603E7</c:v>
                 </c:pt>
-                <c:pt idx="59" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="59" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.28458992831778E7</c:v>
                 </c:pt>
-                <c:pt idx="60" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="60" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.34006414202392E7</c:v>
                 </c:pt>
-                <c:pt idx="61" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="61" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.38033799768333E7</c:v>
                 </c:pt>
-                <c:pt idx="62" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="62" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.45809005423714E7</c:v>
                 </c:pt>
-                <c:pt idx="63" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="63" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.41887988358856E7</c:v>
                 </c:pt>
-                <c:pt idx="64" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="64" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.37850028632028E7</c:v>
                 </c:pt>
-                <c:pt idx="65" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="65" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.406670845526E7</c:v>
                 </c:pt>
-                <c:pt idx="66" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="66" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.44230709625902E7</c:v>
                 </c:pt>
-                <c:pt idx="67" formatCode="_ * #\ ##0_ ;_ * \-#\ ##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="67" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>1.48643374613695E7</c:v>
                 </c:pt>
               </c:numCache>
@@ -2785,11 +2804,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2066150280"/>
-        <c:axId val="2066153224"/>
+        <c:axId val="-2143011480"/>
+        <c:axId val="-2143008504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2066150280"/>
+        <c:axId val="-2143011480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2798,7 +2817,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066153224"/>
+        <c:crossAx val="-2143008504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2806,7 +2825,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2066153224"/>
+        <c:axId val="-2143008504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2817,13 +2836,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066150280"/>
+        <c:crossAx val="-2143011480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3332,47 +3352,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
+      <selection pane="bottomRight" activeCell="I26" sqref="F26:I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1" t="s">
         <v>211</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>212</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G1" t="s">
+        <v>236</v>
+      </c>
+      <c r="H1" t="s">
+        <v>237</v>
+      </c>
+      <c r="I1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J1" t="s">
         <v>213</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>214</v>
       </c>
-      <c r="G1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
+        <v>216</v>
+      </c>
+      <c r="M1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1946</v>
       </c>
@@ -3389,22 +3421,34 @@
         <v>0.22679934864156337</v>
       </c>
       <c r="E2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I2" t="s">
+        <v>215</v>
+      </c>
+      <c r="J2" t="s">
+        <v>215</v>
+      </c>
+      <c r="K2" t="s">
+        <v>215</v>
+      </c>
+      <c r="L2" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="M2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>1947</v>
       </c>
@@ -3421,22 +3465,34 @@
         <v>0.24260125204275501</v>
       </c>
       <c r="E3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I3" t="s">
+        <v>215</v>
+      </c>
+      <c r="J3" t="s">
+        <v>215</v>
+      </c>
+      <c r="K3" t="s">
+        <v>215</v>
+      </c>
+      <c r="L3" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="M3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>1948</v>
       </c>
@@ -3453,22 +3509,34 @@
         <v>0.26422995305021169</v>
       </c>
       <c r="E4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I4" t="s">
+        <v>215</v>
+      </c>
+      <c r="J4" t="s">
+        <v>215</v>
+      </c>
+      <c r="K4" t="s">
+        <v>215</v>
+      </c>
+      <c r="L4" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="M4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>1949</v>
       </c>
@@ -3485,22 +3553,34 @@
         <v>0.28587680381348152</v>
       </c>
       <c r="E5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I5" t="s">
+        <v>215</v>
+      </c>
+      <c r="J5" t="s">
+        <v>215</v>
+      </c>
+      <c r="K5" t="s">
+        <v>215</v>
+      </c>
+      <c r="L5" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="M5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>1950</v>
       </c>
@@ -3517,22 +3597,34 @@
         <v>0.3033310609839055</v>
       </c>
       <c r="E6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H6" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I6" t="s">
+        <v>215</v>
+      </c>
+      <c r="J6" t="s">
+        <v>215</v>
+      </c>
+      <c r="K6" t="s">
+        <v>215</v>
+      </c>
+      <c r="L6" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="M6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>1951</v>
       </c>
@@ -3549,22 +3641,34 @@
         <v>0.31902188787952046</v>
       </c>
       <c r="E7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H7" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I7" t="s">
+        <v>215</v>
+      </c>
+      <c r="J7" t="s">
+        <v>215</v>
+      </c>
+      <c r="K7" t="s">
+        <v>215</v>
+      </c>
+      <c r="L7" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="M7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>1952</v>
       </c>
@@ -3581,22 +3685,34 @@
         <v>0.33768782274803277</v>
       </c>
       <c r="E8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H8" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I8" t="s">
+        <v>215</v>
+      </c>
+      <c r="J8" t="s">
+        <v>215</v>
+      </c>
+      <c r="K8" t="s">
+        <v>215</v>
+      </c>
+      <c r="L8" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="M8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>1953</v>
       </c>
@@ -3613,22 +3729,34 @@
         <v>0.36016593232754646</v>
       </c>
       <c r="E9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H9" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I9" t="s">
+        <v>215</v>
+      </c>
+      <c r="J9" t="s">
+        <v>215</v>
+      </c>
+      <c r="K9" t="s">
+        <v>215</v>
+      </c>
+      <c r="L9" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="M9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>1954</v>
       </c>
@@ -3645,22 +3773,34 @@
         <v>0.38246254434892835</v>
       </c>
       <c r="E10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H10" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I10" t="s">
+        <v>215</v>
+      </c>
+      <c r="J10" t="s">
+        <v>215</v>
+      </c>
+      <c r="K10" t="s">
+        <v>215</v>
+      </c>
+      <c r="L10" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="M10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>1955</v>
       </c>
@@ -3677,22 +3817,34 @@
         <v>0.40271984980714071</v>
       </c>
       <c r="E11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H11" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I11" t="s">
+        <v>215</v>
+      </c>
+      <c r="J11" t="s">
+        <v>215</v>
+      </c>
+      <c r="K11" t="s">
+        <v>215</v>
+      </c>
+      <c r="L11" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="M11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>1956</v>
       </c>
@@ -3709,22 +3861,34 @@
         <v>0.42096253237008951</v>
       </c>
       <c r="E12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H12" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I12" t="s">
+        <v>215</v>
+      </c>
+      <c r="J12" t="s">
+        <v>215</v>
+      </c>
+      <c r="K12" t="s">
+        <v>215</v>
+      </c>
+      <c r="L12" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="M12" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>1957</v>
       </c>
@@ -3741,22 +3905,34 @@
         <v>0.4405904042967006</v>
       </c>
       <c r="E13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H13" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I13" t="s">
+        <v>215</v>
+      </c>
+      <c r="J13" t="s">
+        <v>215</v>
+      </c>
+      <c r="K13" t="s">
+        <v>215</v>
+      </c>
+      <c r="L13" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="M13" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14">
         <v>1958</v>
       </c>
@@ -3773,22 +3949,34 @@
         <v>0.46439562402127443</v>
       </c>
       <c r="E14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H14" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I14" t="s">
+        <v>215</v>
+      </c>
+      <c r="J14" t="s">
+        <v>215</v>
+      </c>
+      <c r="K14" t="s">
+        <v>215</v>
+      </c>
+      <c r="L14" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="M14" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15">
         <v>1959</v>
       </c>
@@ -3805,22 +3993,34 @@
         <v>0.48492444982645205</v>
       </c>
       <c r="E15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H15" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I15" t="s">
+        <v>215</v>
+      </c>
+      <c r="J15" t="s">
+        <v>215</v>
+      </c>
+      <c r="K15" t="s">
+        <v>215</v>
+      </c>
+      <c r="L15" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="M15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16">
         <v>1960</v>
       </c>
@@ -3837,22 +4037,34 @@
         <v>0.50562751328743627</v>
       </c>
       <c r="E16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H16" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I16" t="s">
+        <v>215</v>
+      </c>
+      <c r="J16" t="s">
+        <v>215</v>
+      </c>
+      <c r="K16" t="s">
+        <v>215</v>
+      </c>
+      <c r="L16" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="M16" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17">
         <v>1961</v>
       </c>
@@ -3869,22 +4081,34 @@
         <v>0.52389124956712829</v>
       </c>
       <c r="E17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H17" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I17" t="s">
+        <v>215</v>
+      </c>
+      <c r="J17" t="s">
+        <v>215</v>
+      </c>
+      <c r="K17" t="s">
+        <v>215</v>
+      </c>
+      <c r="L17" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="M17" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18">
         <v>1962</v>
       </c>
@@ -3901,22 +4125,34 @@
         <v>0.54041260928875468</v>
       </c>
       <c r="E18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H18" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I18" t="s">
+        <v>215</v>
+      </c>
+      <c r="J18" t="s">
+        <v>215</v>
+      </c>
+      <c r="K18" t="s">
+        <v>215</v>
+      </c>
+      <c r="L18" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="M18" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19">
         <v>1963</v>
       </c>
@@ -3933,22 +4169,34 @@
         <v>0.56220393210829744</v>
       </c>
       <c r="E19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H19" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I19" t="s">
+        <v>215</v>
+      </c>
+      <c r="J19" t="s">
+        <v>215</v>
+      </c>
+      <c r="K19" t="s">
+        <v>215</v>
+      </c>
+      <c r="L19" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="M19" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20">
         <v>1964</v>
       </c>
@@ -3965,22 +4213,34 @@
         <v>0.5914054372312475</v>
       </c>
       <c r="E20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H20" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I20" t="s">
+        <v>215</v>
+      </c>
+      <c r="J20" t="s">
+        <v>215</v>
+      </c>
+      <c r="K20" t="s">
+        <v>215</v>
+      </c>
+      <c r="L20" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="M20" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21">
         <v>1965</v>
       </c>
@@ -3997,22 +4257,34 @@
         <v>0.62842658314875033</v>
       </c>
       <c r="E21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H21" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I21" t="s">
+        <v>215</v>
+      </c>
+      <c r="J21" t="s">
+        <v>215</v>
+      </c>
+      <c r="K21" t="s">
+        <v>215</v>
+      </c>
+      <c r="L21" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="M21" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22">
         <v>1966</v>
       </c>
@@ -4029,22 +4301,34 @@
         <v>0.66330315391936712</v>
       </c>
       <c r="E22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H22" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I22" t="s">
+        <v>215</v>
+      </c>
+      <c r="J22" t="s">
+        <v>215</v>
+      </c>
+      <c r="K22" t="s">
+        <v>215</v>
+      </c>
+      <c r="L22" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="M22" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23">
         <v>1967</v>
       </c>
@@ -4061,22 +4345,34 @@
         <v>0.69764612186907637</v>
       </c>
       <c r="E23" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F23" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G23" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H23" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I23" t="s">
+        <v>215</v>
+      </c>
+      <c r="J23" t="s">
+        <v>215</v>
+      </c>
+      <c r="K23" t="s">
+        <v>215</v>
+      </c>
+      <c r="L23" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="M23" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24">
         <v>1968</v>
       </c>
@@ -4093,22 +4389,34 @@
         <v>0.73256480007317981</v>
       </c>
       <c r="E24" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F24" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G24" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H24" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I24" t="s">
+        <v>215</v>
+      </c>
+      <c r="J24" t="s">
+        <v>215</v>
+      </c>
+      <c r="K24" t="s">
+        <v>215</v>
+      </c>
+      <c r="L24" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="M24" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25">
         <v>1969</v>
       </c>
@@ -4125,22 +4433,34 @@
         <v>0.77404062205747082</v>
       </c>
       <c r="E25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H25" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I25" t="s">
+        <v>215</v>
+      </c>
+      <c r="J25" t="s">
+        <v>215</v>
+      </c>
+      <c r="K25" t="s">
+        <v>215</v>
+      </c>
+      <c r="L25" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="M25" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26">
         <v>1970</v>
       </c>
@@ -4160,20 +4480,36 @@
         <f>'labour '!E33/'labour '!$E$36</f>
         <v>0.91028898317353013</v>
       </c>
-      <c r="F26" t="s">
-        <v>216</v>
-      </c>
-      <c r="G26" t="s">
-        <v>216</v>
-      </c>
-      <c r="H26" t="s">
-        <v>219</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="F26">
+        <f>'labour '!B33/'labour '!$B$36</f>
+        <v>0.92333577712232928</v>
+      </c>
+      <c r="G26">
+        <f>'labour '!D33/'labour '!$D$36</f>
+        <v>0.92333577712232928</v>
+      </c>
+      <c r="H26">
+        <f>'labour '!E33/'labour '!$E$36</f>
+        <v>0.91028898317353013</v>
+      </c>
+      <c r="I26">
+        <f>'labour '!F33/'labour '!$F$36</f>
+        <v>0.91028898317353013</v>
+      </c>
+      <c r="J26" t="s">
+        <v>215</v>
+      </c>
+      <c r="K26" t="s">
+        <v>215</v>
+      </c>
+      <c r="L26" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="M26" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27">
         <v>1971</v>
       </c>
@@ -4193,20 +4529,36 @@
         <f>'labour '!E34/'labour '!$E$36</f>
         <v>0.93703340039849192</v>
       </c>
-      <c r="F27" t="s">
-        <v>216</v>
-      </c>
-      <c r="G27" t="s">
-        <v>216</v>
-      </c>
-      <c r="H27" t="s">
-        <v>219</v>
-      </c>
-      <c r="I27" t="s">
+      <c r="F27">
+        <f>'labour '!B34/'labour '!$B$36</f>
+        <v>0.9445901877653603</v>
+      </c>
+      <c r="G27">
+        <f>'labour '!D34/'labour '!$D$36</f>
+        <v>0.9445901877653603</v>
+      </c>
+      <c r="H27">
+        <f>'labour '!E34/'labour '!$E$36</f>
+        <v>0.93703340039849192</v>
+      </c>
+      <c r="I27">
+        <f>'labour '!F34/'labour '!$F$36</f>
+        <v>0.93703340039849203</v>
+      </c>
+      <c r="J27" t="s">
+        <v>215</v>
+      </c>
+      <c r="K27" t="s">
+        <v>215</v>
+      </c>
+      <c r="L27" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="M27" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28">
         <v>1972</v>
       </c>
@@ -4226,20 +4578,36 @@
         <f>'labour '!E35/'labour '!$E$36</f>
         <v>0.95822256873969847</v>
       </c>
-      <c r="F28" t="s">
-        <v>216</v>
-      </c>
-      <c r="G28" t="s">
-        <v>216</v>
-      </c>
-      <c r="H28" t="s">
-        <v>219</v>
-      </c>
-      <c r="I28" t="s">
+      <c r="F28">
+        <f>'labour '!B35/'labour '!$B$36</f>
+        <v>0.96118443852064028</v>
+      </c>
+      <c r="G28">
+        <f>'labour '!D35/'labour '!$D$36</f>
+        <v>0.96118443852064039</v>
+      </c>
+      <c r="H28">
+        <f>'labour '!E35/'labour '!$E$36</f>
+        <v>0.95822256873969847</v>
+      </c>
+      <c r="I28">
+        <f>'labour '!F35/'labour '!$F$36</f>
+        <v>0.95822256873969847</v>
+      </c>
+      <c r="J28" t="s">
+        <v>215</v>
+      </c>
+      <c r="K28" t="s">
+        <v>215</v>
+      </c>
+      <c r="L28" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="M28" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29">
         <v>1973</v>
       </c>
@@ -4260,21 +4628,37 @@
         <v>1</v>
       </c>
       <c r="F29">
+        <f>'labour '!B36/'labour '!$B$36</f>
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <f>'labour '!D36/'labour '!$D$36</f>
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <f>'labour '!E36/'labour '!$E$36</f>
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <f>'labour '!F36/'labour '!$F$36</f>
+        <v>1</v>
+      </c>
+      <c r="J29">
         <f>'Energy data'!K16/'Energy data'!$K$16</f>
         <v>1</v>
       </c>
-      <c r="G29">
+      <c r="K29">
         <f>'Energy data'!R16/'Energy data'!$R$16</f>
         <v>1</v>
       </c>
-      <c r="H29" t="s">
-        <v>219</v>
-      </c>
-      <c r="I29" t="s">
+      <c r="L29" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="M29" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30">
         <v>1974</v>
       </c>
@@ -4295,21 +4679,37 @@
         <v>1.0382444840804939</v>
       </c>
       <c r="F30">
+        <f>'labour '!B37/'labour '!$B$36</f>
+        <v>1.0358570789501769</v>
+      </c>
+      <c r="G30">
+        <f>'labour '!D37/'labour '!$D$36</f>
+        <v>1.0358570789501769</v>
+      </c>
+      <c r="H30">
+        <f>'labour '!E37/'labour '!$E$36</f>
+        <v>1.0382444840804939</v>
+      </c>
+      <c r="I30">
+        <f>'labour '!F37/'labour '!$F$36</f>
+        <v>1.0382444840804939</v>
+      </c>
+      <c r="J30">
         <f>'Energy data'!K17/'Energy data'!$K$16</f>
         <v>1.029990951006162</v>
       </c>
-      <c r="G30">
+      <c r="K30">
         <f>'Energy data'!R17/'Energy data'!$R$16</f>
         <v>1.0051975702924416</v>
       </c>
-      <c r="H30" t="s">
-        <v>219</v>
-      </c>
-      <c r="I30" t="s">
+      <c r="L30" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="M30" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31">
         <v>1975</v>
       </c>
@@ -4330,21 +4730,37 @@
         <v>1.0727206861973357</v>
       </c>
       <c r="F31">
+        <f>'labour '!B38/'labour '!$B$36</f>
+        <v>1.0680120517764264</v>
+      </c>
+      <c r="G31">
+        <f>'labour '!D38/'labour '!$D$36</f>
+        <v>1.0680120517764264</v>
+      </c>
+      <c r="H31">
+        <f>'labour '!E38/'labour '!$E$36</f>
+        <v>1.0727206861973357</v>
+      </c>
+      <c r="I31">
+        <f>'labour '!F38/'labour '!$F$36</f>
+        <v>1.0727206861973357</v>
+      </c>
+      <c r="J31">
         <f>'Energy data'!K18/'Energy data'!$K$16</f>
         <v>1.1190589046408412</v>
       </c>
-      <c r="G31">
+      <c r="K31">
         <f>'Energy data'!R18/'Energy data'!$R$16</f>
         <v>1.0780261757154486</v>
       </c>
-      <c r="H31" t="s">
-        <v>219</v>
-      </c>
-      <c r="I31" t="s">
+      <c r="L31" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="M31" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32">
         <v>1976</v>
       </c>
@@ -4365,21 +4781,37 @@
         <v>1.0866430331832257</v>
       </c>
       <c r="F32">
+        <f>'labour '!B39/'labour '!$B$36</f>
+        <v>1.0768993110404073</v>
+      </c>
+      <c r="G32">
+        <f>'labour '!D39/'labour '!$D$36</f>
+        <v>1.0768993110404073</v>
+      </c>
+      <c r="H32">
+        <f>'labour '!E39/'labour '!$E$36</f>
+        <v>1.0866430331832257</v>
+      </c>
+      <c r="I32">
+        <f>'labour '!F39/'labour '!$F$36</f>
+        <v>1.0866430331832257</v>
+      </c>
+      <c r="J32">
         <f>'Energy data'!K19/'Energy data'!$K$16</f>
         <v>1.168009652260094</v>
       </c>
-      <c r="G32">
+      <c r="K32">
         <f>'Energy data'!R19/'Energy data'!$R$16</f>
         <v>1.1149101383931368</v>
       </c>
-      <c r="H32" t="s">
-        <v>219</v>
-      </c>
-      <c r="I32" t="s">
+      <c r="L32" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="M32" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33">
         <v>1977</v>
       </c>
@@ -4400,21 +4832,37 @@
         <v>1.0788515234614313</v>
       </c>
       <c r="F33">
+        <f>'labour '!B40/'labour '!$B$36</f>
+        <v>1.0623062619489441</v>
+      </c>
+      <c r="G33">
+        <f>'labour '!D40/'labour '!$D$36</f>
+        <v>1.0623062619489441</v>
+      </c>
+      <c r="H33">
+        <f>'labour '!E40/'labour '!$E$36</f>
+        <v>1.0788515234614313</v>
+      </c>
+      <c r="I33">
+        <f>'labour '!F40/'labour '!$F$36</f>
+        <v>1.0788515234614313</v>
+      </c>
+      <c r="J33">
         <f>'Energy data'!K20/'Energy data'!$K$16</f>
         <v>1.1740423148188048</v>
       </c>
-      <c r="G33">
+      <c r="K33">
         <f>'Energy data'!R20/'Energy data'!$R$16</f>
         <v>1.089172772246227</v>
       </c>
-      <c r="H33" t="s">
-        <v>219</v>
-      </c>
-      <c r="I33" t="s">
+      <c r="L33" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="M33" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34">
         <v>1978</v>
       </c>
@@ -4435,21 +4883,37 @@
         <v>1.0876250373653398</v>
       </c>
       <c r="F34">
+        <f>'labour '!B41/'labour '!$B$36</f>
+        <v>1.0643549715500999</v>
+      </c>
+      <c r="G34">
+        <f>'labour '!D41/'labour '!$D$36</f>
+        <v>1.0643549715500999</v>
+      </c>
+      <c r="H34">
+        <f>'labour '!E41/'labour '!$E$36</f>
+        <v>1.0876250373653398</v>
+      </c>
+      <c r="I34">
+        <f>'labour '!F41/'labour '!$F$36</f>
+        <v>1.0876250373653398</v>
+      </c>
+      <c r="J34">
         <f>'Energy data'!K21/'Energy data'!$K$16</f>
         <v>1.075537553324428</v>
       </c>
-      <c r="G34">
+      <c r="K34">
         <f>'Energy data'!R21/'Energy data'!$R$16</f>
         <v>1.1509174024672801</v>
       </c>
-      <c r="H34" t="s">
-        <v>219</v>
-      </c>
-      <c r="I34" t="s">
+      <c r="L34" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="M34" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35">
         <v>1979</v>
       </c>
@@ -4470,21 +4934,37 @@
         <v>1.1073602082196052</v>
       </c>
       <c r="F35">
+        <f>'labour '!B42/'labour '!$B$36</f>
+        <v>1.0791226334849746</v>
+      </c>
+      <c r="G35">
+        <f>'labour '!D42/'labour '!$D$36</f>
+        <v>1.0791226334849746</v>
+      </c>
+      <c r="H35">
+        <f>'labour '!E42/'labour '!$E$36</f>
+        <v>1.1073602082196052</v>
+      </c>
+      <c r="I35">
+        <f>'labour '!F42/'labour '!$F$36</f>
+        <v>1.1073602082196055</v>
+      </c>
+      <c r="J35">
         <f>'Energy data'!K22/'Energy data'!$K$16</f>
         <v>1.0948851639591504</v>
       </c>
-      <c r="G35">
+      <c r="K35">
         <f>'Energy data'!R22/'Energy data'!$R$16</f>
         <v>1.1403343978959233</v>
       </c>
-      <c r="H35" t="s">
-        <v>219</v>
-      </c>
-      <c r="I35" t="s">
+      <c r="L35" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="M35" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36">
         <v>1980</v>
       </c>
@@ -4505,21 +4985,37 @@
         <v>1.1471964646370654</v>
       </c>
       <c r="F36">
+        <f>'labour '!B43/'labour '!$B$36</f>
+        <v>1.1151765261466215</v>
+      </c>
+      <c r="G36">
+        <f>'labour '!D43/'labour '!$D$36</f>
+        <v>1.1151765261466215</v>
+      </c>
+      <c r="H36">
+        <f>'labour '!E43/'labour '!$E$36</f>
+        <v>1.1471964646370654</v>
+      </c>
+      <c r="I36">
+        <f>'labour '!F43/'labour '!$F$36</f>
+        <v>1.1471964646370656</v>
+      </c>
+      <c r="J36">
         <f>'Energy data'!K23/'Energy data'!$K$16</f>
         <v>1.1518076442452707</v>
       </c>
-      <c r="G36">
+      <c r="K36">
         <f>'Energy data'!R23/'Energy data'!$R$16</f>
         <v>1.1834178721272464</v>
       </c>
-      <c r="H36" t="s">
-        <v>219</v>
-      </c>
-      <c r="I36" t="s">
+      <c r="L36" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="M36" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37">
         <v>1981</v>
       </c>
@@ -4540,21 +5036,37 @@
         <v>1.1833235328591227</v>
       </c>
       <c r="F37">
+        <f>'labour '!B44/'labour '!$B$36</f>
+        <v>1.1481994435684739</v>
+      </c>
+      <c r="G37">
+        <f>'labour '!D44/'labour '!$D$36</f>
+        <v>1.1481994435684741</v>
+      </c>
+      <c r="H37">
+        <f>'labour '!E44/'labour '!$E$36</f>
+        <v>1.1833235328591227</v>
+      </c>
+      <c r="I37">
+        <f>'labour '!F44/'labour '!$F$36</f>
+        <v>1.1833235328591225</v>
+      </c>
+      <c r="J37">
         <f>'Energy data'!K24/'Energy data'!$K$16</f>
         <v>1.2102382901710691</v>
       </c>
-      <c r="G37">
+      <c r="K37">
         <f>'Energy data'!R24/'Energy data'!$R$16</f>
         <v>1.2435969691276849</v>
       </c>
-      <c r="H37" t="s">
-        <v>219</v>
-      </c>
-      <c r="I37" t="s">
+      <c r="L37" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="M37" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38">
         <v>1982</v>
       </c>
@@ -4575,21 +5087,37 @@
         <v>1.2014983241337824</v>
       </c>
       <c r="F38">
+        <f>'labour '!B45/'labour '!$B$36</f>
+        <v>1.1610506301282266</v>
+      </c>
+      <c r="G38">
+        <f>'labour '!D45/'labour '!$D$36</f>
+        <v>1.1610506301282266</v>
+      </c>
+      <c r="H38">
+        <f>'labour '!E45/'labour '!$E$36</f>
+        <v>1.2014983241337824</v>
+      </c>
+      <c r="I38">
+        <f>'labour '!F45/'labour '!$F$36</f>
+        <v>1.2014983241337827</v>
+      </c>
+      <c r="J38">
         <f>'Energy data'!K25/'Energy data'!$K$16</f>
         <v>1.2000689447149568</v>
       </c>
-      <c r="G38">
+      <c r="K38">
         <f>'Energy data'!R25/'Energy data'!$R$16</f>
         <v>1.1981965057298516</v>
       </c>
-      <c r="H38" t="s">
-        <v>219</v>
-      </c>
-      <c r="I38" t="s">
+      <c r="L38" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="M38" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39">
         <v>1983</v>
       </c>
@@ -4610,21 +5138,37 @@
         <v>1.200218407432375</v>
       </c>
       <c r="F39">
+        <f>'labour '!B46/'labour '!$B$36</f>
+        <v>1.1527824606649568</v>
+      </c>
+      <c r="G39">
+        <f>'labour '!D46/'labour '!$D$36</f>
+        <v>1.1527824606649568</v>
+      </c>
+      <c r="H39">
+        <f>'labour '!E46/'labour '!$E$36</f>
+        <v>1.200218407432375</v>
+      </c>
+      <c r="I39">
+        <f>'labour '!F46/'labour '!$F$36</f>
+        <v>1.200218407432375</v>
+      </c>
+      <c r="J39">
         <f>'Energy data'!K26/'Energy data'!$K$16</f>
         <v>1.1808075149739305</v>
       </c>
-      <c r="G39">
+      <c r="K39">
         <f>'Energy data'!R26/'Energy data'!$R$16</f>
         <v>1.1678251612499218</v>
       </c>
-      <c r="H39" t="s">
-        <v>219</v>
-      </c>
-      <c r="I39" t="s">
+      <c r="L39" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="M39" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40">
         <v>1984</v>
       </c>
@@ -4645,21 +5189,37 @@
         <v>1.2181828954795768</v>
       </c>
       <c r="F40">
+        <f>'labour '!B47/'labour '!$B$36</f>
+        <v>1.1627715002116374</v>
+      </c>
+      <c r="G40">
+        <f>'labour '!D47/'labour '!$D$36</f>
+        <v>1.1627715002116377</v>
+      </c>
+      <c r="H40">
+        <f>'labour '!E47/'labour '!$E$36</f>
+        <v>1.2181828954795768</v>
+      </c>
+      <c r="I40">
+        <f>'labour '!F47/'labour '!$F$36</f>
+        <v>1.2181828954795768</v>
+      </c>
+      <c r="J40">
         <f>'Energy data'!K27/'Energy data'!$K$16</f>
         <v>1.2652217003490329</v>
       </c>
-      <c r="G40">
+      <c r="K40">
         <f>'Energy data'!R27/'Energy data'!$R$16</f>
         <v>1.2445989103888784</v>
       </c>
-      <c r="H40" t="s">
-        <v>219</v>
-      </c>
-      <c r="I40" t="s">
+      <c r="L40" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="M40" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41">
         <v>1985</v>
       </c>
@@ -4680,21 +5240,37 @@
         <v>1.2225080027933586</v>
       </c>
       <c r="F41">
+        <f>'labour '!B48/'labour '!$B$36</f>
+        <v>1.1581279285886608</v>
+      </c>
+      <c r="G41">
+        <f>'labour '!D48/'labour '!$D$36</f>
+        <v>1.158127928588661</v>
+      </c>
+      <c r="H41">
+        <f>'labour '!E48/'labour '!$E$36</f>
+        <v>1.2225080027933586</v>
+      </c>
+      <c r="I41">
+        <f>'labour '!F48/'labour '!$F$36</f>
+        <v>1.2225080027933586</v>
+      </c>
+      <c r="J41">
         <f>'Energy data'!K28/'Energy data'!$K$16</f>
         <v>1.2770284827853666</v>
       </c>
-      <c r="G41">
+      <c r="K41">
         <f>'Energy data'!R28/'Energy data'!$R$16</f>
         <v>1.2554950216043583</v>
       </c>
-      <c r="H41" t="s">
-        <v>219</v>
-      </c>
-      <c r="I41" t="s">
+      <c r="L41" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="M41" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42">
         <v>1986</v>
       </c>
@@ -4715,21 +5291,37 @@
         <v>1.2397767135468609</v>
       </c>
       <c r="F42">
+        <f>'labour '!B49/'labour '!$B$36</f>
+        <v>1.166588114148096</v>
+      </c>
+      <c r="G42">
+        <f>'labour '!D49/'labour '!$D$36</f>
+        <v>1.1937352865233004</v>
+      </c>
+      <c r="H42">
+        <f>'labour '!E49/'labour '!$E$36</f>
+        <v>1.2397767135468609</v>
+      </c>
+      <c r="I42">
+        <f>'labour '!F49/'labour '!$F$36</f>
+        <v>1.2686270264732862</v>
+      </c>
+      <c r="J42">
         <f>'Energy data'!K29/'Energy data'!$K$16</f>
         <v>1.2796570000430907</v>
       </c>
-      <c r="G42">
+      <c r="K42">
         <f>'Energy data'!R29/'Energy data'!$R$16</f>
         <v>1.2483561901183542</v>
       </c>
-      <c r="H42" t="s">
-        <v>219</v>
-      </c>
-      <c r="I42" t="s">
+      <c r="L42" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="M42" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43">
         <v>1987</v>
       </c>
@@ -4750,21 +5342,37 @@
         <v>1.2591894677176954</v>
       </c>
       <c r="F43">
+        <f>'labour '!B50/'labour '!$B$36</f>
+        <v>1.1775524204540055</v>
+      </c>
+      <c r="G43">
+        <f>'labour '!D50/'labour '!$D$36</f>
+        <v>1.23299472416431</v>
+      </c>
+      <c r="H43">
+        <f>'labour '!E50/'labour '!$E$36</f>
+        <v>1.2591894677176954</v>
+      </c>
+      <c r="I43">
+        <f>'labour '!F50/'labour '!$F$36</f>
+        <v>1.3184754610080025</v>
+      </c>
+      <c r="J43">
         <f>'Energy data'!K30/'Energy data'!$K$16</f>
         <v>1.3440341276339038</v>
       </c>
-      <c r="G43">
+      <c r="K43">
         <f>'Energy data'!R30/'Energy data'!$R$16</f>
         <v>1.2854906381113407</v>
       </c>
-      <c r="H43" t="s">
-        <v>219</v>
-      </c>
-      <c r="I43" t="s">
+      <c r="L43" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="M43" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44">
         <v>1988</v>
       </c>
@@ -4785,21 +5393,37 @@
         <v>1.2818596722486471</v>
       </c>
       <c r="F44">
+        <f>'labour '!B51/'labour '!$B$36</f>
+        <v>1.191707536862461</v>
+      </c>
+      <c r="G44">
+        <f>'labour '!D51/'labour '!$D$36</f>
+        <v>1.2768536998738151</v>
+      </c>
+      <c r="H44">
+        <f>'labour '!E51/'labour '!$E$36</f>
+        <v>1.2818596722486471</v>
+      </c>
+      <c r="I44">
+        <f>'labour '!F51/'labour '!$F$36</f>
+        <v>1.3734471039253175</v>
+      </c>
+      <c r="J44">
         <f>'Energy data'!K31/'Energy data'!$K$16</f>
         <v>1.3825569871159566</v>
       </c>
-      <c r="G44">
+      <c r="K44">
         <f>'Energy data'!R31/'Energy data'!$R$16</f>
         <v>1.3523702172960108</v>
       </c>
-      <c r="H44" t="s">
-        <v>219</v>
-      </c>
-      <c r="I44" t="s">
+      <c r="L44" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="M44" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45">
         <v>1989</v>
       </c>
@@ -4820,21 +5444,37 @@
         <v>1.2992227845397488</v>
       </c>
       <c r="F45">
+        <f>'labour '!B52/'labour '!$B$36</f>
+        <v>1.1991033083406899</v>
+      </c>
+      <c r="G45">
+        <f>'labour '!D52/'labour '!$D$36</f>
+        <v>1.3146754069565121</v>
+      </c>
+      <c r="H45">
+        <f>'labour '!E52/'labour '!$E$36</f>
+        <v>1.2992227845397488</v>
+      </c>
+      <c r="I45">
+        <f>'labour '!F52/'labour '!$F$36</f>
+        <v>1.4244446088265426</v>
+      </c>
+      <c r="J45">
         <f>'Energy data'!K32/'Energy data'!$K$16</f>
         <v>1.4230620071530142</v>
       </c>
-      <c r="G45">
+      <c r="K45">
         <f>'Energy data'!R32/'Energy data'!$R$16</f>
         <v>1.3832425324065374</v>
       </c>
-      <c r="H45" t="s">
-        <v>219</v>
-      </c>
-      <c r="I45" t="s">
+      <c r="L45" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="M45" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46">
         <v>1990</v>
       </c>
@@ -4855,21 +5495,37 @@
         <v>1.3080902446782243</v>
       </c>
       <c r="F46">
+        <f>'labour '!B53/'labour '!$B$36</f>
+        <v>1.1955063273323741</v>
+      </c>
+      <c r="G46">
+        <f>'labour '!D53/'labour '!$D$36</f>
+        <v>1.3412332183437703</v>
+      </c>
+      <c r="H46">
+        <f>'labour '!E53/'labour '!$E$36</f>
+        <v>1.3080902446782243</v>
+      </c>
+      <c r="I46">
+        <f>'labour '!F53/'labour '!$F$36</f>
+        <v>1.4675406132468694</v>
+      </c>
+      <c r="J46">
         <f>'Energy data'!K33/'Energy data'!$K$16</f>
         <v>1.4841211703365365</v>
       </c>
-      <c r="G46">
+      <c r="K46">
         <f>'Energy data'!R33/'Energy data'!$R$16</f>
         <v>1.3929488383743502</v>
       </c>
-      <c r="H46" t="s">
-        <v>219</v>
-      </c>
-      <c r="I46" t="s">
+      <c r="L46" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="M46" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47">
         <v>1991</v>
       </c>
@@ -4890,21 +5546,37 @@
         <v>1.3054791434282975</v>
       </c>
       <c r="F47">
+        <f>'labour '!B54/'labour '!$B$36</f>
+        <v>1.1786460081415622</v>
+      </c>
+      <c r="G47">
+        <f>'labour '!D54/'labour '!$D$36</f>
+        <v>1.3530887903214037</v>
+      </c>
+      <c r="H47">
+        <f>'labour '!E54/'labour '!$E$36</f>
+        <v>1.3054791434282975</v>
+      </c>
+      <c r="I47">
+        <f>'labour '!F54/'labour '!$F$36</f>
+        <v>1.4986935710718148</v>
+      </c>
+      <c r="J47">
         <f>'Energy data'!K34/'Energy data'!$K$16</f>
         <v>1.4777868746498903</v>
       </c>
-      <c r="G47">
+      <c r="K47">
         <f>'Energy data'!R34/'Energy data'!$R$16</f>
         <v>1.3740998183981465</v>
       </c>
-      <c r="H47" t="s">
-        <v>219</v>
-      </c>
-      <c r="I47" t="s">
+      <c r="L47" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="M47" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48">
         <v>1992</v>
       </c>
@@ -4925,21 +5597,37 @@
         <v>1.3045697437852499</v>
       </c>
       <c r="F48">
+        <f>'labour '!B55/'labour '!$B$36</f>
+        <v>1.162983015105215</v>
+      </c>
+      <c r="G48">
+        <f>'labour '!D55/'labour '!$D$36</f>
+        <v>1.366176350054793</v>
+      </c>
+      <c r="H48">
+        <f>'labour '!E55/'labour '!$E$36</f>
+        <v>1.3045697437852499</v>
+      </c>
+      <c r="I48">
+        <f>'labour '!F55/'labour '!$F$36</f>
+        <v>1.5325007397422798</v>
+      </c>
+      <c r="J48">
         <f>'Energy data'!K35/'Energy data'!$K$16</f>
         <v>1.4669280820442108</v>
       </c>
-      <c r="G48">
+      <c r="K48">
         <f>'Energy data'!R35/'Energy data'!$R$16</f>
         <v>1.332957605360386</v>
       </c>
-      <c r="H48" t="s">
-        <v>219</v>
-      </c>
-      <c r="I48" t="s">
+      <c r="L48" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="M48" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
       <c r="A49">
         <v>1993</v>
       </c>
@@ -4960,21 +5648,37 @@
         <v>1.3071701709914374</v>
       </c>
       <c r="F49">
+        <f>'labour '!B56/'labour '!$B$36</f>
+        <v>1.1493052921992661</v>
+      </c>
+      <c r="G49">
+        <f>'labour '!D56/'labour '!$D$36</f>
+        <v>1.3815266971440769</v>
+      </c>
+      <c r="H49">
+        <f>'labour '!E56/'labour '!$E$36</f>
+        <v>1.3071701709914374</v>
+      </c>
+      <c r="I49">
+        <f>'labour '!F56/'labour '!$F$36</f>
+        <v>1.5712887612997728</v>
+      </c>
+      <c r="J49">
         <f>'Energy data'!K36/'Energy data'!$K$16</f>
         <v>1.5544447795923646</v>
       </c>
-      <c r="G49">
+      <c r="K49">
         <f>'Energy data'!R36/'Energy data'!$R$16</f>
         <v>1.3320809067568415</v>
       </c>
-      <c r="H49" t="s">
-        <v>219</v>
-      </c>
-      <c r="I49" t="s">
+      <c r="L49" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="M49" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
       <c r="A50">
         <v>1994</v>
       </c>
@@ -4995,21 +5699,37 @@
         <v>1.3141509044561606</v>
       </c>
       <c r="F50">
+        <f>'labour '!B57/'labour '!$B$36</f>
+        <v>1.1446165767907364</v>
+      </c>
+      <c r="G50">
+        <f>'labour '!D57/'labour '!$D$36</f>
+        <v>1.4079083704654676</v>
+      </c>
+      <c r="H50">
+        <f>'labour '!E57/'labour '!$E$36</f>
+        <v>1.3141509044561606</v>
+      </c>
+      <c r="I50">
+        <f>'labour '!F57/'labour '!$F$36</f>
+        <v>1.6164400341170797</v>
+      </c>
+      <c r="J50">
         <f>'Energy data'!K37/'Energy data'!$K$16</f>
         <v>1.6020597233593314</v>
       </c>
-      <c r="G50">
+      <c r="K50">
         <f>'Energy data'!R37/'Energy data'!$R$16</f>
         <v>1.3687143841192309</v>
       </c>
-      <c r="H50" t="s">
-        <v>219</v>
-      </c>
-      <c r="I50" t="s">
+      <c r="L50" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="M50" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
       <c r="A51">
         <v>1995</v>
       </c>
@@ -5030,21 +5750,37 @@
         <v>1.3290565756177866</v>
       </c>
       <c r="F51">
+        <f>'labour '!B58/'labour '!$B$36</f>
+        <v>1.1458454489284469</v>
+      </c>
+      <c r="G51">
+        <f>'labour '!D58/'labour '!$D$36</f>
+        <v>1.4422179226039296</v>
+      </c>
+      <c r="H51">
+        <f>'labour '!E58/'labour '!$E$36</f>
+        <v>1.3290565756177866</v>
+      </c>
+      <c r="I51">
+        <f>'labour '!F58/'labour '!$F$36</f>
+        <v>1.6728165349900268</v>
+      </c>
+      <c r="J51">
         <f>'Energy data'!K38/'Energy data'!$K$16</f>
         <v>1.7083638557331844</v>
       </c>
-      <c r="G51">
+      <c r="K51">
         <f>'Energy data'!R38/'Energy data'!$R$16</f>
         <v>1.4638361826037947</v>
       </c>
-      <c r="H51" t="s">
-        <v>219</v>
-      </c>
-      <c r="I51" t="s">
+      <c r="L51" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="M51" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
       <c r="A52">
         <v>1996</v>
       </c>
@@ -5065,21 +5801,37 @@
         <v>1.3478509939555294</v>
       </c>
       <c r="F52">
+        <f>'labour '!B59/'labour '!$B$36</f>
+        <v>1.1560121643684795</v>
+      </c>
+      <c r="G52">
+        <f>'labour '!D59/'labour '!$D$36</f>
+        <v>1.4550142549848288</v>
+      </c>
+      <c r="H52">
+        <f>'labour '!E59/'labour '!$E$36</f>
+        <v>1.3478509939555294</v>
+      </c>
+      <c r="I52">
+        <f>'labour '!F59/'labour '!$F$36</f>
+        <v>1.6964721222221069</v>
+      </c>
+      <c r="J52">
         <f>'Energy data'!K39/'Energy data'!$K$16</f>
         <v>1.7874779161459904</v>
       </c>
-      <c r="G52">
+      <c r="K52">
         <f>'Energy data'!R39/'Energy data'!$R$16</f>
         <v>1.5423633289498402</v>
       </c>
-      <c r="H52" t="s">
-        <v>219</v>
-      </c>
-      <c r="I52" t="s">
+      <c r="L52" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="M52" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
       <c r="A53">
         <v>1997</v>
       </c>
@@ -5100,21 +5852,37 @@
         <v>1.3516425773294416</v>
       </c>
       <c r="F53">
+        <f>'labour '!B60/'labour '!$B$36</f>
+        <v>1.1528869079700799</v>
+      </c>
+      <c r="G53">
+        <f>'labour '!D60/'labour '!$D$36</f>
+        <v>1.4510806522509527</v>
+      </c>
+      <c r="H53">
+        <f>'labour '!E60/'labour '!$E$36</f>
+        <v>1.3516425773294416</v>
+      </c>
+      <c r="I53">
+        <f>'labour '!F60/'labour '!$F$36</f>
+        <v>1.7012443971410474</v>
+      </c>
+      <c r="J53">
         <f>'Energy data'!K40/'Energy data'!$K$16</f>
         <v>1.9469987503770414</v>
       </c>
-      <c r="G53">
+      <c r="K53">
         <f>'Energy data'!R40/'Energy data'!$R$16</f>
         <v>1.6019788339908574</v>
       </c>
-      <c r="H53" t="s">
-        <v>219</v>
-      </c>
-      <c r="I53" t="s">
+      <c r="L53" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="M53" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54">
         <v>1998</v>
       </c>
@@ -5135,21 +5903,37 @@
         <v>1.3374286861121705</v>
       </c>
       <c r="F54">
+        <f>'labour '!B61/'labour '!$B$36</f>
+        <v>1.1355485379690513</v>
+      </c>
+      <c r="G54">
+        <f>'labour '!D61/'labour '!$D$36</f>
+        <v>1.4292577196839067</v>
+      </c>
+      <c r="H54">
+        <f>'labour '!E61/'labour '!$E$36</f>
+        <v>1.3374286861121705</v>
+      </c>
+      <c r="I54">
+        <f>'labour '!F61/'labour '!$F$36</f>
+        <v>1.683354088563515</v>
+      </c>
+      <c r="J54">
         <f>'Energy data'!K41/'Energy data'!$K$16</f>
         <v>1.8943422243288659</v>
       </c>
-      <c r="G54">
+      <c r="K54">
         <f>'Energy data'!R41/'Energy data'!$R$16</f>
         <v>1.5893293255682888</v>
       </c>
-      <c r="H54" t="s">
-        <v>219</v>
-      </c>
-      <c r="I54" t="s">
+      <c r="L54" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="M54" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
       <c r="A55">
         <v>1999</v>
       </c>
@@ -5170,21 +5954,37 @@
         <v>1.3341025545279603</v>
       </c>
       <c r="F55">
+        <f>'labour '!B62/'labour '!$B$36</f>
+        <v>1.1294418119467229</v>
+      </c>
+      <c r="G55">
+        <f>'labour '!D62/'labour '!$D$36</f>
+        <v>1.4215714913831619</v>
+      </c>
+      <c r="H55">
+        <f>'labour '!E62/'labour '!$E$36</f>
+        <v>1.3341025545279603</v>
+      </c>
+      <c r="I55">
+        <f>'labour '!F62/'labour '!$F$36</f>
+        <v>1.6791676543562029</v>
+      </c>
+      <c r="J55">
         <f>'Energy data'!K42/'Energy data'!$K$16</f>
         <v>1.8629292885767232</v>
       </c>
-      <c r="G55">
+      <c r="K55">
         <f>'Energy data'!R42/'Energy data'!$R$16</f>
         <v>1.5453065314045964</v>
       </c>
-      <c r="H55" t="s">
-        <v>219</v>
-      </c>
-      <c r="I55" t="s">
+      <c r="L55" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="M55" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56">
         <v>2000</v>
       </c>
@@ -5205,21 +6005,37 @@
         <v>1.320319309319465</v>
       </c>
       <c r="F56">
+        <f>'labour '!B63/'labour '!$B$36</f>
+        <v>1.1206713526740804</v>
+      </c>
+      <c r="G56">
+        <f>'labour '!D63/'labour '!$D$36</f>
+        <v>1.4105325562769466</v>
+      </c>
+      <c r="H56">
+        <f>'labour '!E63/'labour '!$E$36</f>
+        <v>1.320319309319465</v>
+      </c>
+      <c r="I56">
+        <f>'labour '!F63/'labour '!$F$36</f>
+        <v>1.6618193782078563</v>
+      </c>
+      <c r="J56">
         <f>'Energy data'!K43/'Energy data'!$K$16</f>
         <v>1.9042961175507396</v>
       </c>
-      <c r="G56">
+      <c r="K56">
         <f>'Energy data'!R43/'Energy data'!$R$16</f>
         <v>1.5663472978896613</v>
       </c>
-      <c r="H56" t="s">
-        <v>219</v>
-      </c>
-      <c r="I56" t="s">
+      <c r="L56" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="M56" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57">
         <v>2001</v>
       </c>
@@ -5240,21 +6056,37 @@
         <v>1.2687051452501636</v>
       </c>
       <c r="F57">
+        <f>'labour '!B64/'labour '!$B$36</f>
+        <v>1.1096287388075015</v>
+      </c>
+      <c r="G57">
+        <f>'labour '!D64/'labour '!$D$36</f>
+        <v>1.3966337746867525</v>
+      </c>
+      <c r="H57">
+        <f>'labour '!E64/'labour '!$E$36</f>
+        <v>1.2687051452501636</v>
+      </c>
+      <c r="I57">
+        <f>'labour '!F64/'labour '!$F$36</f>
+        <v>1.5968552309482249</v>
+      </c>
+      <c r="J57">
         <f>'Energy data'!K44/'Energy data'!$K$16</f>
         <v>1.8556470030594225</v>
       </c>
-      <c r="G57">
+      <c r="K57">
         <f>'Energy data'!R44/'Energy data'!$R$16</f>
         <v>1.5470599286116851</v>
       </c>
-      <c r="H57" t="s">
-        <v>219</v>
-      </c>
-      <c r="I57" t="s">
+      <c r="L57" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="M57" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58">
         <v>2002</v>
       </c>
@@ -5275,21 +6107,37 @@
         <v>1.2565404162051708</v>
       </c>
       <c r="F58">
+        <f>'labour '!B65/'labour '!$B$36</f>
+        <v>1.1549048899999546</v>
+      </c>
+      <c r="G58">
+        <f>'labour '!D65/'labour '!$D$36</f>
+        <v>1.4536205845373702</v>
+      </c>
+      <c r="H58">
+        <f>'labour '!E65/'labour '!$E$36</f>
+        <v>1.2565404162051708</v>
+      </c>
+      <c r="I58">
+        <f>'labour '!F65/'labour '!$F$36</f>
+        <v>1.5815440995310555</v>
+      </c>
+      <c r="J58">
         <f>'Energy data'!K45/'Energy data'!$K$16</f>
         <v>1.952859051148361</v>
       </c>
-      <c r="G58">
+      <c r="K58">
         <f>'Energy data'!R45/'Energy data'!$R$16</f>
         <v>1.6297200826601539</v>
       </c>
-      <c r="H58" t="s">
-        <v>219</v>
-      </c>
-      <c r="I58" t="s">
+      <c r="L58" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="M58" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
       <c r="A59">
         <v>2003</v>
       </c>
@@ -5310,21 +6158,37 @@
         <v>1.2841687463472171</v>
       </c>
       <c r="F59">
+        <f>'labour '!B66/'labour '!$B$36</f>
+        <v>1.1445141682138202</v>
+      </c>
+      <c r="G59">
+        <f>'labour '!D66/'labour '!$D$36</f>
+        <v>1.4405423066572527</v>
+      </c>
+      <c r="H59">
+        <f>'labour '!E66/'labour '!$E$36</f>
+        <v>1.2841687463472171</v>
+      </c>
+      <c r="I59">
+        <f>'labour '!F66/'labour '!$F$36</f>
+        <v>1.6163184863733122</v>
+      </c>
+      <c r="J59">
         <f>'Energy data'!K46/'Energy data'!$K$16</f>
         <v>1.9979747489981472</v>
       </c>
-      <c r="G59">
+      <c r="K59">
         <f>'Energy data'!R46/'Energy data'!$R$16</f>
         <v>1.6952846139395077</v>
       </c>
-      <c r="H59" t="s">
-        <v>219</v>
-      </c>
-      <c r="I59" t="s">
+      <c r="L59" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="M59" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60">
         <v>2004</v>
       </c>
@@ -5345,21 +6209,37 @@
         <v>1.3178330948213797</v>
       </c>
       <c r="F60">
+        <f>'labour '!B67/'labour '!$B$36</f>
+        <v>1.152710785725148</v>
+      </c>
+      <c r="G60">
+        <f>'labour '!D67/'labour '!$D$36</f>
+        <v>1.450858976056796</v>
+      </c>
+      <c r="H60">
+        <f>'labour '!E67/'labour '!$E$36</f>
+        <v>1.3178330948213797</v>
+      </c>
+      <c r="I60">
+        <f>'labour '!F67/'labour '!$F$36</f>
+        <v>1.6586901053099019</v>
+      </c>
+      <c r="J60">
         <f>'Energy data'!K47/'Energy data'!$K$16</f>
         <v>2.0863101650364113</v>
       </c>
-      <c r="G60">
+      <c r="K60">
         <f>'Energy data'!R47/'Energy data'!$R$16</f>
         <v>1.7300394514371593</v>
       </c>
-      <c r="H60" t="s">
-        <v>219</v>
-      </c>
-      <c r="I60" t="s">
+      <c r="L60" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="M60" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
       <c r="A61">
         <v>2005</v>
       </c>
@@ -5380,21 +6260,37 @@
         <v>1.3502139920474661</v>
       </c>
       <c r="F61">
+        <f>'labour '!B68/'labour '!$B$36</f>
+        <v>1.1489795614486409</v>
+      </c>
+      <c r="G61">
+        <f>'labour '!D68/'labour '!$D$36</f>
+        <v>1.4461626720920113</v>
+      </c>
+      <c r="H61">
+        <f>'labour '!E68/'labour '!$E$36</f>
+        <v>1.3502139920474661</v>
+      </c>
+      <c r="I61">
+        <f>'labour '!F68/'labour '!$F$36</f>
+        <v>1.6994463088390341</v>
+      </c>
+      <c r="J61">
         <f>'Energy data'!K48/'Energy data'!$K$16</f>
         <v>2.1118197095703879</v>
       </c>
-      <c r="G61">
+      <c r="K61">
         <f>'Energy data'!R48/'Energy data'!$R$16</f>
         <v>1.7472603168639236</v>
       </c>
-      <c r="H61" t="s">
-        <v>219</v>
-      </c>
-      <c r="I61" t="s">
+      <c r="L61" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="M61" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
       <c r="A62">
         <v>2006</v>
       </c>
@@ -5415,21 +6311,37 @@
         <v>1.40852213995732</v>
       </c>
       <c r="F62">
+        <f>'labour '!B69/'labour '!$B$36</f>
+        <v>1.1955812540833528</v>
+      </c>
+      <c r="G62">
+        <f>'labour '!D69/'labour '!$D$36</f>
+        <v>1.5109391270348216</v>
+      </c>
+      <c r="H62">
+        <f>'labour '!E69/'labour '!$E$36</f>
+        <v>1.40852213995732</v>
+      </c>
+      <c r="I62">
+        <f>'labour '!F69/'labour '!$F$36</f>
+        <v>1.7800473245024295</v>
+      </c>
+      <c r="J62">
         <f>'Energy data'!K49/'Energy data'!$K$16</f>
         <v>2.0354634377558498</v>
       </c>
-      <c r="G62">
+      <c r="K62">
         <f>'Energy data'!R49/'Energy data'!$R$16</f>
         <v>1.7419375039138327</v>
       </c>
-      <c r="H62" t="s">
-        <v>219</v>
-      </c>
-      <c r="I62" t="s">
+      <c r="L62" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="M62" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
       <c r="A63">
         <v>2007</v>
       </c>
@@ -5450,21 +6362,37 @@
         <v>1.4508534102143162</v>
       </c>
       <c r="F63">
+        <f>'labour '!B70/'labour '!$B$36</f>
+        <v>1.212780495787539</v>
+      </c>
+      <c r="G63">
+        <f>'labour '!D70/'labour '!$D$36</f>
+        <v>1.5389095734457872</v>
+      </c>
+      <c r="H63">
+        <f>'labour '!E70/'labour '!$E$36</f>
+        <v>1.4508534102143162</v>
+      </c>
+      <c r="I63">
+        <f>'labour '!F70/'labour '!$F$36</f>
+        <v>1.8410027291834183</v>
+      </c>
+      <c r="J63">
         <f>'Energy data'!K50/'Energy data'!$K$16</f>
         <v>2.1911923126642825</v>
       </c>
-      <c r="G63">
+      <c r="K63">
         <f>'Energy data'!R50/'Energy data'!$R$16</f>
         <v>1.9090112092178595</v>
       </c>
-      <c r="H63" t="s">
-        <v>219</v>
-      </c>
-      <c r="I63" t="s">
+      <c r="L63" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="64" spans="1:9">
+      <c r="M63" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
       <c r="A64">
         <v>2008</v>
       </c>
@@ -5485,21 +6413,37 @@
         <v>1.5325774782263533</v>
       </c>
       <c r="F64">
+        <f>'labour '!B71/'labour '!$B$36</f>
+        <v>1.2059356699631989</v>
+      </c>
+      <c r="G64">
+        <f>'labour '!D71/'labour '!$D$36</f>
+        <v>1.5364487035352723</v>
+      </c>
+      <c r="H64">
+        <f>'labour '!E71/'labour '!$E$36</f>
+        <v>1.5325774782263533</v>
+      </c>
+      <c r="I64">
+        <f>'labour '!F71/'labour '!$F$36</f>
+        <v>1.952613840139662</v>
+      </c>
+      <c r="J64">
         <f>'Energy data'!K51/'Energy data'!$K$16</f>
         <v>2.3412332485887881</v>
       </c>
-      <c r="G64">
+      <c r="K64">
         <f>'Energy data'!R51/'Energy data'!$R$16</f>
         <v>1.8536539545369148</v>
       </c>
-      <c r="H64" t="s">
-        <v>219</v>
-      </c>
-      <c r="I64" t="s">
+      <c r="L64" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="M64" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
       <c r="A65">
         <v>2009</v>
       </c>
@@ -5520,21 +6464,37 @@
         <v>1.4913642319808285</v>
       </c>
       <c r="F65">
+        <f>'labour '!B72/'labour '!$B$36</f>
+        <v>1.1642851762823798</v>
+      </c>
+      <c r="G65">
+        <f>'labour '!D72/'labour '!$D$36</f>
+        <v>1.4894170421978703</v>
+      </c>
+      <c r="H65">
+        <f>'labour '!E72/'labour '!$E$36</f>
+        <v>1.4913642319808285</v>
+      </c>
+      <c r="I65">
+        <f>'labour '!F72/'labour '!$F$36</f>
+        <v>1.9078343935711586</v>
+      </c>
+      <c r="J65">
         <f>'Energy data'!K52/'Energy data'!$K$16</f>
         <v>2.21209117938553</v>
       </c>
-      <c r="G65">
+      <c r="K65">
         <f>'Energy data'!R52/'Energy data'!$R$16</f>
         <v>1.8879704427327944</v>
       </c>
-      <c r="H65" t="s">
-        <v>219</v>
-      </c>
-      <c r="I65" t="s">
+      <c r="L65" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="66" spans="1:9">
+      <c r="M65" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
       <c r="A66">
         <v>2010</v>
       </c>
@@ -5555,21 +6515,37 @@
         <v>1.4489218182400709</v>
       </c>
       <c r="F66">
+        <f>'labour '!B73/'labour '!$B$36</f>
+        <v>1.1457617583390758</v>
+      </c>
+      <c r="G66">
+        <f>'labour '!D73/'labour '!$D$36</f>
+        <v>1.4716830918670798</v>
+      </c>
+      <c r="H66">
+        <f>'labour '!E73/'labour '!$E$36</f>
+        <v>1.4489218182400709</v>
+      </c>
+      <c r="I66">
+        <f>'labour '!F73/'labour '!$F$36</f>
+        <v>1.8610795183392495</v>
+      </c>
+      <c r="J66">
         <f>'Energy data'!K53/'Energy data'!$K$16</f>
         <v>2.2680225793941484</v>
       </c>
-      <c r="G66">
+      <c r="K66">
         <f>'Energy data'!R53/'Energy data'!$R$16</f>
         <v>1.8787651073955787</v>
       </c>
-      <c r="H66" t="s">
-        <v>219</v>
-      </c>
-      <c r="I66" t="s">
+      <c r="L66" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="67" spans="1:9">
+      <c r="M66" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
       <c r="A67">
         <v>2011</v>
       </c>
@@ -5590,21 +6566,37 @@
         <v>1.4785314877267177</v>
       </c>
       <c r="F67">
+        <f>'labour '!B74/'labour '!$B$36</f>
+        <v>1.1603708644982589</v>
+      </c>
+      <c r="G67">
+        <f>'labour '!D74/'labour '!$D$36</f>
+        <v>1.4904478781459722</v>
+      </c>
+      <c r="H67">
+        <f>'labour '!E74/'labour '!$E$36</f>
+        <v>1.4785314877267177</v>
+      </c>
+      <c r="I67">
+        <f>'labour '!F74/'labour '!$F$36</f>
+        <v>1.8991119012688729</v>
+      </c>
+      <c r="J67">
         <f>'Energy data'!K54/'Energy data'!$K$16</f>
         <v>2.2600077562804324</v>
       </c>
-      <c r="G67">
+      <c r="K67">
         <f>'Energy data'!R54/'Energy data'!$R$16</f>
         <v>1.9590456509487129</v>
       </c>
-      <c r="H67" t="s">
-        <v>219</v>
-      </c>
-      <c r="I67" t="s">
+      <c r="L67" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="68" spans="1:9">
+      <c r="M67" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13">
       <c r="A68">
         <v>2012</v>
       </c>
@@ -5624,20 +6616,36 @@
         <f>'labour '!E75/'labour '!$E$36</f>
         <v>1.5159882381675731</v>
       </c>
-      <c r="F68" t="s">
-        <v>216</v>
-      </c>
-      <c r="G68" t="s">
-        <v>216</v>
-      </c>
-      <c r="H68" t="s">
-        <v>219</v>
-      </c>
-      <c r="I68" t="s">
+      <c r="F68">
+        <f>'labour '!B75/'labour '!$B$36</f>
+        <v>1.1798335520788421</v>
+      </c>
+      <c r="G68">
+        <f>'labour '!D75/'labour '!$D$36</f>
+        <v>1.5154468869068838</v>
+      </c>
+      <c r="H68">
+        <f>'labour '!E75/'labour '!$E$36</f>
+        <v>1.5159882381675731</v>
+      </c>
+      <c r="I68">
+        <f>'labour '!F75/'labour '!$F$36</f>
+        <v>1.9472235317181226</v>
+      </c>
+      <c r="J68" t="s">
+        <v>215</v>
+      </c>
+      <c r="K68" t="s">
+        <v>215</v>
+      </c>
+      <c r="L68" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="69" spans="1:9">
+      <c r="M68" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
       <c r="A69">
         <v>2013</v>
       </c>
@@ -5657,17 +6665,33 @@
         <f>'labour '!E76/'labour '!$E$36</f>
         <v>1.5623691249968692</v>
       </c>
-      <c r="F69" t="s">
-        <v>216</v>
-      </c>
-      <c r="G69" t="s">
-        <v>216</v>
-      </c>
-      <c r="H69" t="s">
-        <v>219</v>
-      </c>
-      <c r="I69" t="s">
+      <c r="F69">
+        <f>'labour '!B76/'labour '!$B$36</f>
+        <v>1.1894539153510799</v>
+      </c>
+      <c r="G69">
+        <f>'labour '!D76/'labour '!$D$36</f>
+        <v>1.5278038414502919</v>
+      </c>
+      <c r="H69">
+        <f>'labour '!E76/'labour '!$E$36</f>
+        <v>1.5623691249968692</v>
+      </c>
+      <c r="I69">
+        <f>'labour '!F76/'labour '!$F$36</f>
+        <v>2.0067978423771065</v>
+      </c>
+      <c r="J69" t="s">
+        <v>215</v>
+      </c>
+      <c r="K69" t="s">
+        <v>215</v>
+      </c>
+      <c r="L69" t="s">
         <v>218</v>
+      </c>
+      <c r="M69" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -13392,11 +14416,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A8:AH76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="D60" sqref="D60"/>
+      <selection pane="bottomRight" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13440,98 +14464,98 @@
         <v>194</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>233</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>195</v>
+        <v>234</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>233</v>
       </c>
       <c r="G8" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3" t="s">
         <v>190</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>49</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>50</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Q8" s="3" t="s">
         <v>191</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="S8" s="3" t="s">
         <v>52</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U8" s="3" t="s">
         <v>53</v>
       </c>
       <c r="V8" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="W8" s="3" t="s">
         <v>54</v>
       </c>
       <c r="X8" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Y8" s="3" t="s">
         <v>55</v>
       </c>
       <c r="Z8" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AA8" s="3" t="s">
         <v>192</v>
       </c>
       <c r="AB8" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AC8" s="3" t="s">
         <v>57</v>
       </c>
       <c r="AD8" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AE8" s="3" t="s">
         <v>193</v>
       </c>
       <c r="AF8" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AG8" s="3" t="s">
         <v>59</v>
       </c>
       <c r="AH8" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:34">
@@ -24097,10 +25121,10 @@
     <row r="2" spans="1:3" ht="24" customHeight="1">
       <c r="A2" s="156"/>
       <c r="B2" s="158" t="s">
+        <v>220</v>
+      </c>
+      <c r="C2" s="158" t="s">
         <v>221</v>
-      </c>
-      <c r="C2" s="158" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -24113,10 +25137,10 @@
         <v>1980</v>
       </c>
       <c r="B4" s="154" t="s">
+        <v>222</v>
+      </c>
+      <c r="C4" s="154" t="s">
         <v>223</v>
-      </c>
-      <c r="C4" s="154" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -24129,10 +25153,10 @@
         <v>1985</v>
       </c>
       <c r="B6" s="154" t="s">
+        <v>222</v>
+      </c>
+      <c r="C6" s="154" t="s">
         <v>223</v>
-      </c>
-      <c r="C6" s="154" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -24145,10 +25169,10 @@
         <v>1990</v>
       </c>
       <c r="B8" s="154" t="s">
+        <v>224</v>
+      </c>
+      <c r="C8" s="154" t="s">
         <v>225</v>
-      </c>
-      <c r="C8" s="154" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -24161,10 +25185,10 @@
         <v>1995</v>
       </c>
       <c r="B10" s="154" t="s">
+        <v>226</v>
+      </c>
+      <c r="C10" s="154" t="s">
         <v>227</v>
-      </c>
-      <c r="C10" s="154" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -24177,10 +25201,10 @@
         <v>2000</v>
       </c>
       <c r="B12" s="154" t="s">
+        <v>226</v>
+      </c>
+      <c r="C12" s="154" t="s">
         <v>227</v>
-      </c>
-      <c r="C12" s="154" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -24193,10 +25217,10 @@
         <v>2005</v>
       </c>
       <c r="B14" s="154" t="s">
+        <v>226</v>
+      </c>
+      <c r="C14" s="154" t="s">
         <v>227</v>
-      </c>
-      <c r="C14" s="154" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -24209,10 +25233,10 @@
         <v>2010</v>
       </c>
       <c r="B16" s="154" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C16" s="154" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -24225,10 +25249,10 @@
         <v>2011</v>
       </c>
       <c r="B18" s="154" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C18" s="154" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -24241,10 +25265,10 @@
         <v>2012</v>
       </c>
       <c r="B20" s="154" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C20" s="154" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -24254,46 +25278,46 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="B26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Changed name of labor time series.
</commit_message>
<xml_diff>
--- a/data/Excel Workbooks/SUN/SUN Data with education.xlsx
+++ b/data/Excel Workbooks/SUN/SUN Data with education.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28160" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Indexed" sheetId="1" r:id="rId1"/>
@@ -800,13 +800,13 @@
     <t>iL_f</t>
   </si>
   <si>
-    <t>iL_f+e</t>
+    <t>iL_fe</t>
   </si>
   <si>
-    <t>iL_f+i</t>
+    <t>iL_fi</t>
   </si>
   <si>
-    <t>iL_f+i+e</t>
+    <t>iL_fie</t>
   </si>
 </sst>
 </file>
@@ -1982,11 +1982,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2146386248"/>
-        <c:axId val="-2146389208"/>
+        <c:axId val="-2146378680"/>
+        <c:axId val="-2143002312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2146386248"/>
+        <c:axId val="-2146378680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1995,7 +1995,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146389208"/>
+        <c:crossAx val="-2143002312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2003,7 +2003,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2146389208"/>
+        <c:axId val="-2143002312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2014,7 +2014,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146386248"/>
+        <c:crossAx val="-2146378680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2804,11 +2804,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2143011480"/>
-        <c:axId val="-2143008504"/>
+        <c:axId val="-2146365624"/>
+        <c:axId val="-2136777096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2143011480"/>
+        <c:axId val="-2146365624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2817,7 +2817,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143008504"/>
+        <c:crossAx val="-2136777096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2825,7 +2825,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2143008504"/>
+        <c:axId val="-2136777096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2836,14 +2836,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143011480"/>
+        <c:crossAx val="-2146365624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3355,10 +3354,10 @@
   <dimension ref="A1:M69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I26" sqref="F26:I69"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -25288,36 +25287,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Changed name of education variables.
</commit_message>
<xml_diff>
--- a/data/Excel Workbooks/SUN/SUN Data with education.xlsx
+++ b/data/Excel Workbooks/SUN/SUN Data with education.xlsx
@@ -797,16 +797,16 @@
     <t>Total form+inf</t>
   </si>
   <si>
-    <t>iL_f</t>
+    <t>iLf</t>
   </si>
   <si>
-    <t>iL_fe</t>
+    <t>iLfe</t>
   </si>
   <si>
-    <t>iL_fi</t>
+    <t>iLfi</t>
   </si>
   <si>
-    <t>iL_fie</t>
+    <t>iLfie</t>
   </si>
 </sst>
 </file>
@@ -1982,11 +1982,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2146378680"/>
-        <c:axId val="-2143002312"/>
+        <c:axId val="-2128445048"/>
+        <c:axId val="-2142932568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2146378680"/>
+        <c:axId val="-2128445048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1995,7 +1995,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143002312"/>
+        <c:crossAx val="-2142932568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2003,7 +2003,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2143002312"/>
+        <c:axId val="-2142932568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2014,7 +2014,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146378680"/>
+        <c:crossAx val="-2128445048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2804,11 +2804,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2146365624"/>
-        <c:axId val="-2136777096"/>
+        <c:axId val="-2136828296"/>
+        <c:axId val="-2136823192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2146365624"/>
+        <c:axId val="-2136828296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2817,7 +2817,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136777096"/>
+        <c:crossAx val="-2136823192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2825,7 +2825,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2136777096"/>
+        <c:axId val="-2136823192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2836,7 +2836,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146365624"/>
+        <c:crossAx val="-2136828296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25287,36 +25287,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Now using formal+informal+education for labor.
</commit_message>
<xml_diff>
--- a/data/Excel Workbooks/SUN/SUN Data with education.xlsx
+++ b/data/Excel Workbooks/SUN/SUN Data with education.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28160" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Indexed" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="239">
   <si>
     <t>Year</t>
   </si>
@@ -1982,11 +1982,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2128445048"/>
-        <c:axId val="-2142932568"/>
+        <c:axId val="-2138795784"/>
+        <c:axId val="-2138792840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2128445048"/>
+        <c:axId val="-2138795784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1995,7 +1995,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142932568"/>
+        <c:crossAx val="-2138792840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2003,7 +2003,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2142932568"/>
+        <c:axId val="-2138792840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2014,7 +2014,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128445048"/>
+        <c:crossAx val="-2138795784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2804,11 +2804,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2136828296"/>
-        <c:axId val="-2136823192"/>
+        <c:axId val="-2138690776"/>
+        <c:axId val="-2138687832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2136828296"/>
+        <c:axId val="-2138690776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2817,7 +2817,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136823192"/>
+        <c:crossAx val="-2138687832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2825,7 +2825,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2136823192"/>
+        <c:axId val="-2138687832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2836,7 +2836,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136828296"/>
+        <c:crossAx val="-2138690776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3354,10 +3354,10 @@
   <dimension ref="A1:M69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3419,8 +3419,9 @@
         <f>'Real capital stock'!B9/'Real capital stock'!$B$36</f>
         <v>0.22679934864156337</v>
       </c>
-      <c r="E2" t="s">
-        <v>215</v>
+      <c r="E2" t="str">
+        <f>I2</f>
+        <v>NA</v>
       </c>
       <c r="F2" t="s">
         <v>215</v>
@@ -3463,8 +3464,9 @@
         <f>'Real capital stock'!B10/'Real capital stock'!$B$36</f>
         <v>0.24260125204275501</v>
       </c>
-      <c r="E3" t="s">
-        <v>215</v>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E66" si="1">I3</f>
+        <v>NA</v>
       </c>
       <c r="F3" t="s">
         <v>215</v>
@@ -3507,8 +3509,9 @@
         <f>'Real capital stock'!B11/'Real capital stock'!$B$36</f>
         <v>0.26422995305021169</v>
       </c>
-      <c r="E4" t="s">
-        <v>215</v>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F4" t="s">
         <v>215</v>
@@ -3551,8 +3554,9 @@
         <f>'Real capital stock'!B12/'Real capital stock'!$B$36</f>
         <v>0.28587680381348152</v>
       </c>
-      <c r="E5" t="s">
-        <v>215</v>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F5" t="s">
         <v>215</v>
@@ -3595,8 +3599,9 @@
         <f>'Real capital stock'!B13/'Real capital stock'!$B$36</f>
         <v>0.3033310609839055</v>
       </c>
-      <c r="E6" t="s">
-        <v>215</v>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F6" t="s">
         <v>215</v>
@@ -3639,8 +3644,9 @@
         <f>'Real capital stock'!B14/'Real capital stock'!$B$36</f>
         <v>0.31902188787952046</v>
       </c>
-      <c r="E7" t="s">
-        <v>215</v>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F7" t="s">
         <v>215</v>
@@ -3683,8 +3689,9 @@
         <f>'Real capital stock'!B15/'Real capital stock'!$B$36</f>
         <v>0.33768782274803277</v>
       </c>
-      <c r="E8" t="s">
-        <v>215</v>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F8" t="s">
         <v>215</v>
@@ -3727,8 +3734,9 @@
         <f>'Real capital stock'!B16/'Real capital stock'!$B$36</f>
         <v>0.36016593232754646</v>
       </c>
-      <c r="E9" t="s">
-        <v>215</v>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F9" t="s">
         <v>215</v>
@@ -3771,8 +3779,9 @@
         <f>'Real capital stock'!B17/'Real capital stock'!$B$36</f>
         <v>0.38246254434892835</v>
       </c>
-      <c r="E10" t="s">
-        <v>215</v>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F10" t="s">
         <v>215</v>
@@ -3815,8 +3824,9 @@
         <f>'Real capital stock'!B18/'Real capital stock'!$B$36</f>
         <v>0.40271984980714071</v>
       </c>
-      <c r="E11" t="s">
-        <v>215</v>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F11" t="s">
         <v>215</v>
@@ -3859,8 +3869,9 @@
         <f>'Real capital stock'!B19/'Real capital stock'!$B$36</f>
         <v>0.42096253237008951</v>
       </c>
-      <c r="E12" t="s">
-        <v>215</v>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F12" t="s">
         <v>215</v>
@@ -3903,8 +3914,9 @@
         <f>'Real capital stock'!B20/'Real capital stock'!$B$36</f>
         <v>0.4405904042967006</v>
       </c>
-      <c r="E13" t="s">
-        <v>215</v>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F13" t="s">
         <v>215</v>
@@ -3947,8 +3959,9 @@
         <f>'Real capital stock'!B21/'Real capital stock'!$B$36</f>
         <v>0.46439562402127443</v>
       </c>
-      <c r="E14" t="s">
-        <v>215</v>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F14" t="s">
         <v>215</v>
@@ -3991,8 +4004,9 @@
         <f>'Real capital stock'!B22/'Real capital stock'!$B$36</f>
         <v>0.48492444982645205</v>
       </c>
-      <c r="E15" t="s">
-        <v>215</v>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F15" t="s">
         <v>215</v>
@@ -4035,8 +4049,9 @@
         <f>'Real capital stock'!B23/'Real capital stock'!$B$36</f>
         <v>0.50562751328743627</v>
       </c>
-      <c r="E16" t="s">
-        <v>215</v>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F16" t="s">
         <v>215</v>
@@ -4079,8 +4094,9 @@
         <f>'Real capital stock'!B24/'Real capital stock'!$B$36</f>
         <v>0.52389124956712829</v>
       </c>
-      <c r="E17" t="s">
-        <v>215</v>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F17" t="s">
         <v>215</v>
@@ -4123,8 +4139,9 @@
         <f>'Real capital stock'!B25/'Real capital stock'!$B$36</f>
         <v>0.54041260928875468</v>
       </c>
-      <c r="E18" t="s">
-        <v>215</v>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F18" t="s">
         <v>215</v>
@@ -4167,8 +4184,9 @@
         <f>'Real capital stock'!B26/'Real capital stock'!$B$36</f>
         <v>0.56220393210829744</v>
       </c>
-      <c r="E19" t="s">
-        <v>215</v>
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F19" t="s">
         <v>215</v>
@@ -4211,8 +4229,9 @@
         <f>'Real capital stock'!B27/'Real capital stock'!$B$36</f>
         <v>0.5914054372312475</v>
       </c>
-      <c r="E20" t="s">
-        <v>215</v>
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F20" t="s">
         <v>215</v>
@@ -4255,8 +4274,9 @@
         <f>'Real capital stock'!B28/'Real capital stock'!$B$36</f>
         <v>0.62842658314875033</v>
       </c>
-      <c r="E21" t="s">
-        <v>215</v>
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F21" t="s">
         <v>215</v>
@@ -4299,8 +4319,9 @@
         <f>'Real capital stock'!B29/'Real capital stock'!$B$36</f>
         <v>0.66330315391936712</v>
       </c>
-      <c r="E22" t="s">
-        <v>215</v>
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F22" t="s">
         <v>215</v>
@@ -4343,8 +4364,9 @@
         <f>'Real capital stock'!B30/'Real capital stock'!$B$36</f>
         <v>0.69764612186907637</v>
       </c>
-      <c r="E23" t="s">
-        <v>215</v>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F23" t="s">
         <v>215</v>
@@ -4387,8 +4409,9 @@
         <f>'Real capital stock'!B31/'Real capital stock'!$B$36</f>
         <v>0.73256480007317981</v>
       </c>
-      <c r="E24" t="s">
-        <v>215</v>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F24" t="s">
         <v>215</v>
@@ -4431,8 +4454,9 @@
         <f>'Real capital stock'!B32/'Real capital stock'!$B$36</f>
         <v>0.77404062205747082</v>
       </c>
-      <c r="E25" t="s">
-        <v>215</v>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
       </c>
       <c r="F25" t="s">
         <v>215</v>
@@ -4476,7 +4500,7 @@
         <v>0.8232453360572487</v>
       </c>
       <c r="E26">
-        <f>'labour '!E33/'labour '!$E$36</f>
+        <f t="shared" si="1"/>
         <v>0.91028898317353013</v>
       </c>
       <c r="F26">
@@ -4525,8 +4549,8 @@
         <v>0.87928670007673715</v>
       </c>
       <c r="E27">
-        <f>'labour '!E34/'labour '!$E$36</f>
-        <v>0.93703340039849192</v>
+        <f t="shared" si="1"/>
+        <v>0.93703340039849203</v>
       </c>
       <c r="F27">
         <f>'labour '!B34/'labour '!$B$36</f>
@@ -4574,7 +4598,7 @@
         <v>0.93907562567653213</v>
       </c>
       <c r="E28">
-        <f>'labour '!E35/'labour '!$E$36</f>
+        <f t="shared" si="1"/>
         <v>0.95822256873969847</v>
       </c>
       <c r="F28">
@@ -4623,7 +4647,7 @@
         <v>1</v>
       </c>
       <c r="E29">
-        <f>'labour '!E36/'labour '!$E$36</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F29">
@@ -4662,7 +4686,7 @@
         <v>1974</v>
       </c>
       <c r="B30">
-        <f t="shared" ref="B30:B69" si="1">A30-$A$29</f>
+        <f t="shared" ref="B30:B69" si="2">A30-$A$29</f>
         <v>1</v>
       </c>
       <c r="C30">
@@ -4674,7 +4698,7 @@
         <v>1.0644846304237823</v>
       </c>
       <c r="E30">
-        <f>'labour '!E37/'labour '!$E$36</f>
+        <f t="shared" si="1"/>
         <v>1.0382444840804939</v>
       </c>
       <c r="F30">
@@ -4713,7 +4737,7 @@
         <v>1975</v>
       </c>
       <c r="B31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="C31">
@@ -4725,7 +4749,7 @@
         <v>1.136540612982593</v>
       </c>
       <c r="E31">
-        <f>'labour '!E38/'labour '!$E$36</f>
+        <f t="shared" si="1"/>
         <v>1.0727206861973357</v>
       </c>
       <c r="F31">
@@ -4764,7 +4788,7 @@
         <v>1976</v>
       </c>
       <c r="B32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C32">
@@ -4776,7 +4800,7 @@
         <v>1.2041121538750819</v>
       </c>
       <c r="E32">
-        <f>'labour '!E39/'labour '!$E$36</f>
+        <f t="shared" si="1"/>
         <v>1.0866430331832257</v>
       </c>
       <c r="F32">
@@ -4815,7 +4839,7 @@
         <v>1977</v>
       </c>
       <c r="B33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="C33">
@@ -4827,7 +4851,7 @@
         <v>1.2613949611921922</v>
       </c>
       <c r="E33">
-        <f>'labour '!E40/'labour '!$E$36</f>
+        <f t="shared" si="1"/>
         <v>1.0788515234614313</v>
       </c>
       <c r="F33">
@@ -4866,7 +4890,7 @@
         <v>1978</v>
       </c>
       <c r="B34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="C34">
@@ -4878,7 +4902,7 @@
         <v>1.3100805921757128</v>
       </c>
       <c r="E34">
-        <f>'labour '!E41/'labour '!$E$36</f>
+        <f t="shared" si="1"/>
         <v>1.0876250373653398</v>
       </c>
       <c r="F34">
@@ -4917,7 +4941,7 @@
         <v>1979</v>
       </c>
       <c r="B35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="C35">
@@ -4929,8 +4953,8 @@
         <v>1.359450831948507</v>
       </c>
       <c r="E35">
-        <f>'labour '!E42/'labour '!$E$36</f>
-        <v>1.1073602082196052</v>
+        <f t="shared" si="1"/>
+        <v>1.1073602082196055</v>
       </c>
       <c r="F35">
         <f>'labour '!B42/'labour '!$B$36</f>
@@ -4968,7 +4992,7 @@
         <v>1980</v>
       </c>
       <c r="B36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="C36">
@@ -4980,8 +5004,8 @@
         <v>1.4247964867880667</v>
       </c>
       <c r="E36">
-        <f>'labour '!E43/'labour '!$E$36</f>
-        <v>1.1471964646370654</v>
+        <f t="shared" si="1"/>
+        <v>1.1471964646370656</v>
       </c>
       <c r="F36">
         <f>'labour '!B43/'labour '!$B$36</f>
@@ -5019,7 +5043,7 @@
         <v>1981</v>
       </c>
       <c r="B37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="C37">
@@ -5031,8 +5055,8 @@
         <v>1.4963450021743407</v>
       </c>
       <c r="E37">
-        <f>'labour '!E44/'labour '!$E$36</f>
-        <v>1.1833235328591227</v>
+        <f t="shared" si="1"/>
+        <v>1.1833235328591225</v>
       </c>
       <c r="F37">
         <f>'labour '!B44/'labour '!$B$36</f>
@@ -5070,7 +5094,7 @@
         <v>1982</v>
       </c>
       <c r="B38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="C38">
@@ -5082,8 +5106,8 @@
         <v>1.5569775284243326</v>
       </c>
       <c r="E38">
-        <f>'labour '!E45/'labour '!$E$36</f>
-        <v>1.2014983241337824</v>
+        <f t="shared" si="1"/>
+        <v>1.2014983241337827</v>
       </c>
       <c r="F38">
         <f>'labour '!B45/'labour '!$B$36</f>
@@ -5121,7 +5145,7 @@
         <v>1983</v>
       </c>
       <c r="B39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="C39">
@@ -5133,7 +5157,7 @@
         <v>1.6083014079128579</v>
       </c>
       <c r="E39">
-        <f>'labour '!E46/'labour '!$E$36</f>
+        <f t="shared" si="1"/>
         <v>1.200218407432375</v>
       </c>
       <c r="F39">
@@ -5172,7 +5196,7 @@
         <v>1984</v>
       </c>
       <c r="B40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="C40">
@@ -5184,7 +5208,7 @@
         <v>1.6527719396063245</v>
       </c>
       <c r="E40">
-        <f>'labour '!E47/'labour '!$E$36</f>
+        <f t="shared" si="1"/>
         <v>1.2181828954795768</v>
       </c>
       <c r="F40">
@@ -5223,7 +5247,7 @@
         <v>1985</v>
       </c>
       <c r="B41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="C41">
@@ -5235,7 +5259,7 @@
         <v>1.686669149553262</v>
       </c>
       <c r="E41">
-        <f>'labour '!E48/'labour '!$E$36</f>
+        <f t="shared" si="1"/>
         <v>1.2225080027933586</v>
       </c>
       <c r="F41">
@@ -5274,7 +5298,7 @@
         <v>1986</v>
       </c>
       <c r="B42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="C42">
@@ -5286,8 +5310,8 @@
         <v>1.7000934349429262</v>
       </c>
       <c r="E42">
-        <f>'labour '!E49/'labour '!$E$36</f>
-        <v>1.2397767135468609</v>
+        <f t="shared" si="1"/>
+        <v>1.2686270264732862</v>
       </c>
       <c r="F42">
         <f>'labour '!B49/'labour '!$B$36</f>
@@ -5325,7 +5349,7 @@
         <v>1987</v>
       </c>
       <c r="B43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="C43">
@@ -5337,8 +5361,8 @@
         <v>1.7079050898449213</v>
       </c>
       <c r="E43">
-        <f>'labour '!E50/'labour '!$E$36</f>
-        <v>1.2591894677176954</v>
+        <f t="shared" si="1"/>
+        <v>1.3184754610080025</v>
       </c>
       <c r="F43">
         <f>'labour '!B50/'labour '!$B$36</f>
@@ -5376,7 +5400,7 @@
         <v>1988</v>
       </c>
       <c r="B44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="C44">
@@ -5388,8 +5412,8 @@
         <v>1.7262682867864696</v>
       </c>
       <c r="E44">
-        <f>'labour '!E51/'labour '!$E$36</f>
-        <v>1.2818596722486471</v>
+        <f t="shared" si="1"/>
+        <v>1.3734471039253175</v>
       </c>
       <c r="F44">
         <f>'labour '!B51/'labour '!$B$36</f>
@@ -5427,7 +5451,7 @@
         <v>1989</v>
       </c>
       <c r="B45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="C45">
@@ -5439,8 +5463,8 @@
         <v>1.7525498591941944</v>
       </c>
       <c r="E45">
-        <f>'labour '!E52/'labour '!$E$36</f>
-        <v>1.2992227845397488</v>
+        <f t="shared" si="1"/>
+        <v>1.4244446088265426</v>
       </c>
       <c r="F45">
         <f>'labour '!B52/'labour '!$B$36</f>
@@ -5478,7 +5502,7 @@
         <v>1990</v>
       </c>
       <c r="B46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="C46">
@@ -5490,8 +5514,8 @@
         <v>1.7768596421303748</v>
       </c>
       <c r="E46">
-        <f>'labour '!E53/'labour '!$E$36</f>
-        <v>1.3080902446782243</v>
+        <f t="shared" si="1"/>
+        <v>1.4675406132468694</v>
       </c>
       <c r="F46">
         <f>'labour '!B53/'labour '!$B$36</f>
@@ -5529,7 +5553,7 @@
         <v>1991</v>
       </c>
       <c r="B47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="C47">
@@ -5541,8 +5565,8 @@
         <v>1.7930564842180614</v>
       </c>
       <c r="E47">
-        <f>'labour '!E54/'labour '!$E$36</f>
-        <v>1.3054791434282975</v>
+        <f t="shared" si="1"/>
+        <v>1.4986935710718148</v>
       </c>
       <c r="F47">
         <f>'labour '!B54/'labour '!$B$36</f>
@@ -5580,7 +5604,7 @@
         <v>1992</v>
       </c>
       <c r="B48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="C48">
@@ -5592,8 +5616,8 @@
         <v>1.8020732829060517</v>
       </c>
       <c r="E48">
-        <f>'labour '!E55/'labour '!$E$36</f>
-        <v>1.3045697437852499</v>
+        <f t="shared" si="1"/>
+        <v>1.5325007397422798</v>
       </c>
       <c r="F48">
         <f>'labour '!B55/'labour '!$B$36</f>
@@ -5631,7 +5655,7 @@
         <v>1993</v>
       </c>
       <c r="B49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="C49">
@@ -5643,8 +5667,8 @@
         <v>1.8089360685741334</v>
       </c>
       <c r="E49">
-        <f>'labour '!E56/'labour '!$E$36</f>
-        <v>1.3071701709914374</v>
+        <f t="shared" si="1"/>
+        <v>1.5712887612997728</v>
       </c>
       <c r="F49">
         <f>'labour '!B56/'labour '!$B$36</f>
@@ -5682,7 +5706,7 @@
         <v>1994</v>
       </c>
       <c r="B50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="C50">
@@ -5694,8 +5718,8 @@
         <v>1.8212866144098898</v>
       </c>
       <c r="E50">
-        <f>'labour '!E57/'labour '!$E$36</f>
-        <v>1.3141509044561606</v>
+        <f t="shared" si="1"/>
+        <v>1.6164400341170797</v>
       </c>
       <c r="F50">
         <f>'labour '!B57/'labour '!$B$36</f>
@@ -5733,7 +5757,7 @@
         <v>1995</v>
       </c>
       <c r="B51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="C51">
@@ -5745,8 +5769,8 @@
         <v>1.8406611157453487</v>
       </c>
       <c r="E51">
-        <f>'labour '!E58/'labour '!$E$36</f>
-        <v>1.3290565756177866</v>
+        <f t="shared" si="1"/>
+        <v>1.6728165349900268</v>
       </c>
       <c r="F51">
         <f>'labour '!B58/'labour '!$B$36</f>
@@ -5784,7 +5808,7 @@
         <v>1996</v>
       </c>
       <c r="B52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="C52">
@@ -5796,8 +5820,8 @@
         <v>1.8671067619456247</v>
       </c>
       <c r="E52">
-        <f>'labour '!E59/'labour '!$E$36</f>
-        <v>1.3478509939555294</v>
+        <f t="shared" si="1"/>
+        <v>1.6964721222221069</v>
       </c>
       <c r="F52">
         <f>'labour '!B59/'labour '!$B$36</f>
@@ -5835,7 +5859,7 @@
         <v>1997</v>
       </c>
       <c r="B53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="C53">
@@ -5847,8 +5871,8 @@
         <v>1.8961979165532308</v>
       </c>
       <c r="E53">
-        <f>'labour '!E60/'labour '!$E$36</f>
-        <v>1.3516425773294416</v>
+        <f t="shared" si="1"/>
+        <v>1.7012443971410474</v>
       </c>
       <c r="F53">
         <f>'labour '!B60/'labour '!$B$36</f>
@@ -5886,7 +5910,7 @@
         <v>1998</v>
       </c>
       <c r="B54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="C54">
@@ -5898,8 +5922,8 @@
         <v>1.9267308877626361</v>
       </c>
       <c r="E54">
-        <f>'labour '!E61/'labour '!$E$36</f>
-        <v>1.3374286861121705</v>
+        <f t="shared" si="1"/>
+        <v>1.683354088563515</v>
       </c>
       <c r="F54">
         <f>'labour '!B61/'labour '!$B$36</f>
@@ -5937,7 +5961,7 @@
         <v>1999</v>
       </c>
       <c r="B55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="C55">
@@ -5949,8 +5973,8 @@
         <v>1.9412942518271359</v>
       </c>
       <c r="E55">
-        <f>'labour '!E62/'labour '!$E$36</f>
-        <v>1.3341025545279603</v>
+        <f t="shared" si="1"/>
+        <v>1.6791676543562029</v>
       </c>
       <c r="F55">
         <f>'labour '!B62/'labour '!$B$36</f>
@@ -5988,7 +6012,7 @@
         <v>2000</v>
       </c>
       <c r="B56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="C56">
@@ -6000,8 +6024,8 @@
         <v>1.9569669289669376</v>
       </c>
       <c r="E56">
-        <f>'labour '!E63/'labour '!$E$36</f>
-        <v>1.320319309319465</v>
+        <f t="shared" si="1"/>
+        <v>1.6618193782078563</v>
       </c>
       <c r="F56">
         <f>'labour '!B63/'labour '!$B$36</f>
@@ -6039,7 +6063,7 @@
         <v>2001</v>
       </c>
       <c r="B57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="C57">
@@ -6051,8 +6075,8 @@
         <v>1.972721643003015</v>
       </c>
       <c r="E57">
-        <f>'labour '!E64/'labour '!$E$36</f>
-        <v>1.2687051452501636</v>
+        <f t="shared" si="1"/>
+        <v>1.5968552309482249</v>
       </c>
       <c r="F57">
         <f>'labour '!B64/'labour '!$B$36</f>
@@ -6090,7 +6114,7 @@
         <v>2002</v>
       </c>
       <c r="B58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="C58">
@@ -6102,8 +6126,8 @@
         <v>1.9890019739674423</v>
       </c>
       <c r="E58">
-        <f>'labour '!E65/'labour '!$E$36</f>
-        <v>1.2565404162051708</v>
+        <f t="shared" si="1"/>
+        <v>1.5815440995310555</v>
       </c>
       <c r="F58">
         <f>'labour '!B65/'labour '!$B$36</f>
@@ -6141,7 +6165,7 @@
         <v>2003</v>
       </c>
       <c r="B59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="C59">
@@ -6153,8 +6177,8 @@
         <v>2.0155507107807371</v>
       </c>
       <c r="E59">
-        <f>'labour '!E66/'labour '!$E$36</f>
-        <v>1.2841687463472171</v>
+        <f t="shared" si="1"/>
+        <v>1.6163184863733122</v>
       </c>
       <c r="F59">
         <f>'labour '!B66/'labour '!$B$36</f>
@@ -6192,7 +6216,7 @@
         <v>2004</v>
       </c>
       <c r="B60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="C60">
@@ -6204,8 +6228,8 @@
         <v>2.0571158295636289</v>
       </c>
       <c r="E60">
-        <f>'labour '!E67/'labour '!$E$36</f>
-        <v>1.3178330948213797</v>
+        <f t="shared" si="1"/>
+        <v>1.6586901053099019</v>
       </c>
       <c r="F60">
         <f>'labour '!B67/'labour '!$B$36</f>
@@ -6243,7 +6267,7 @@
         <v>2005</v>
       </c>
       <c r="B61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="C61">
@@ -6255,8 +6279,8 @@
         <v>2.1122910872357124</v>
       </c>
       <c r="E61">
-        <f>'labour '!E68/'labour '!$E$36</f>
-        <v>1.3502139920474661</v>
+        <f t="shared" si="1"/>
+        <v>1.6994463088390341</v>
       </c>
       <c r="F61">
         <f>'labour '!B68/'labour '!$B$36</f>
@@ -6294,7 +6318,7 @@
         <v>2006</v>
       </c>
       <c r="B62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="C62">
@@ -6306,8 +6330,8 @@
         <v>2.1835688082652536</v>
       </c>
       <c r="E62">
-        <f>'labour '!E69/'labour '!$E$36</f>
-        <v>1.40852213995732</v>
+        <f t="shared" si="1"/>
+        <v>1.7800473245024295</v>
       </c>
       <c r="F62">
         <f>'labour '!B69/'labour '!$B$36</f>
@@ -6345,7 +6369,7 @@
         <v>2007</v>
       </c>
       <c r="B63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="C63">
@@ -6357,8 +6381,8 @@
         <v>2.2667070317235951</v>
       </c>
       <c r="E63">
-        <f>'labour '!E70/'labour '!$E$36</f>
-        <v>1.4508534102143162</v>
+        <f t="shared" si="1"/>
+        <v>1.8410027291834183</v>
       </c>
       <c r="F63">
         <f>'labour '!B70/'labour '!$B$36</f>
@@ -6396,7 +6420,7 @@
         <v>2008</v>
       </c>
       <c r="B64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="C64">
@@ -6408,8 +6432,8 @@
         <v>2.382392123296373</v>
       </c>
       <c r="E64">
-        <f>'labour '!E71/'labour '!$E$36</f>
-        <v>1.5325774782263533</v>
+        <f t="shared" si="1"/>
+        <v>1.952613840139662</v>
       </c>
       <c r="F64">
         <f>'labour '!B71/'labour '!$B$36</f>
@@ -6447,7 +6471,7 @@
         <v>2009</v>
       </c>
       <c r="B65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="C65">
@@ -6459,8 +6483,8 @@
         <v>2.4750596945468697</v>
       </c>
       <c r="E65">
-        <f>'labour '!E72/'labour '!$E$36</f>
-        <v>1.4913642319808285</v>
+        <f t="shared" si="1"/>
+        <v>1.9078343935711586</v>
       </c>
       <c r="F65">
         <f>'labour '!B72/'labour '!$B$36</f>
@@ -6498,7 +6522,7 @@
         <v>2010</v>
       </c>
       <c r="B66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="C66">
@@ -6510,8 +6534,8 @@
         <v>2.5547806819807048</v>
       </c>
       <c r="E66">
-        <f>'labour '!E73/'labour '!$E$36</f>
-        <v>1.4489218182400709</v>
+        <f t="shared" si="1"/>
+        <v>1.8610795183392495</v>
       </c>
       <c r="F66">
         <f>'labour '!B73/'labour '!$B$36</f>
@@ -6549,7 +6573,7 @@
         <v>2011</v>
       </c>
       <c r="B67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="C67">
@@ -6561,8 +6585,8 @@
         <v>2.6368001544907216</v>
       </c>
       <c r="E67">
-        <f>'labour '!E74/'labour '!$E$36</f>
-        <v>1.4785314877267177</v>
+        <f t="shared" ref="E67:E69" si="3">I67</f>
+        <v>1.8991119012688729</v>
       </c>
       <c r="F67">
         <f>'labour '!B74/'labour '!$B$36</f>
@@ -6600,7 +6624,7 @@
         <v>2012</v>
       </c>
       <c r="B68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="C68">
@@ -6612,8 +6636,8 @@
         <v>2.7230579579782335</v>
       </c>
       <c r="E68">
-        <f>'labour '!E75/'labour '!$E$36</f>
-        <v>1.5159882381675731</v>
+        <f t="shared" si="3"/>
+        <v>1.9472235317181226</v>
       </c>
       <c r="F68">
         <f>'labour '!B75/'labour '!$B$36</f>
@@ -6649,7 +6673,7 @@
         <v>2013</v>
       </c>
       <c r="B69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="C69">
@@ -6661,8 +6685,8 @@
         <v>2.8152456496850293</v>
       </c>
       <c r="E69">
-        <f>'labour '!E76/'labour '!$E$36</f>
-        <v>1.5623691249968692</v>
+        <f t="shared" si="3"/>
+        <v>2.0067978423771065</v>
       </c>
       <c r="F69">
         <f>'labour '!B76/'labour '!$B$36</f>
@@ -25287,36 +25311,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>